<commit_message>
Gantt chart updates, Flowchart added, Moon and Spacestation copies
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\MoonGame\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8DD4BA-D884-4678-A37A-A3961051FAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A29F1-E95B-4437-B665-7D5B38F1F6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Observatory and stars</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Sliding Doors</t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -789,6 +795,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1158,7 +1170,7 @@
   <dimension ref="A1:BZ48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1254,38 +1266,38 @@
     </row>
     <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
       <c r="AH2" s="12"/>
@@ -1414,43 +1426,43 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="67" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="65" t="s">
+      <c r="I4" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="69" t="s">
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
@@ -1502,42 +1514,42 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="79" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
       <c r="H5" s="19"/>
-      <c r="I5" s="65" t="s">
+      <c r="I5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="80">
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="82">
         <v>44802</v>
       </c>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="68"/>
-      <c r="T5" s="68"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="68"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
       <c r="AB5" s="20"/>
       <c r="AC5" s="18"/>
       <c r="AD5" s="1"/>
@@ -1754,205 +1766,205 @@
     </row>
     <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="73"/>
-      <c r="V8" s="73"/>
-      <c r="W8" s="73"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="73"/>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="73"/>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="73"/>
-      <c r="AD8" s="73"/>
-      <c r="AE8" s="73"/>
-      <c r="AF8" s="73"/>
-      <c r="AG8" s="73"/>
-      <c r="AH8" s="73"/>
-      <c r="AI8" s="73"/>
-      <c r="AJ8" s="73"/>
-      <c r="AK8" s="73"/>
-      <c r="AL8" s="73"/>
-      <c r="AM8" s="74"/>
-      <c r="AN8" s="73"/>
-      <c r="AO8" s="73"/>
-      <c r="AP8" s="73"/>
-      <c r="AQ8" s="73"/>
-      <c r="AR8" s="73"/>
-      <c r="AS8" s="73"/>
-      <c r="AT8" s="73"/>
-      <c r="AU8" s="73"/>
-      <c r="AV8" s="73"/>
-      <c r="AW8" s="73"/>
-      <c r="AX8" s="73"/>
-      <c r="AY8" s="73"/>
-      <c r="AZ8" s="73"/>
-      <c r="BA8" s="73"/>
-      <c r="BB8" s="74"/>
-      <c r="BC8" s="73"/>
-      <c r="BD8" s="73"/>
-      <c r="BE8" s="73"/>
-      <c r="BF8" s="73"/>
-      <c r="BG8" s="73"/>
-      <c r="BH8" s="73"/>
-      <c r="BI8" s="73"/>
-      <c r="BJ8" s="73"/>
-      <c r="BK8" s="73"/>
-      <c r="BL8" s="73"/>
-      <c r="BM8" s="73"/>
-      <c r="BN8" s="73"/>
-      <c r="BO8" s="73"/>
-      <c r="BP8" s="73"/>
-      <c r="BQ8" s="73"/>
-      <c r="BR8" s="73"/>
-      <c r="BS8" s="73"/>
-      <c r="BT8" s="73"/>
-      <c r="BU8" s="73"/>
-      <c r="BV8" s="73"/>
-      <c r="BW8" s="73"/>
-      <c r="BX8" s="73"/>
-      <c r="BY8" s="73"/>
-      <c r="BZ8" s="78"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="75"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="75"/>
+      <c r="X8" s="76"/>
+      <c r="Y8" s="75"/>
+      <c r="Z8" s="75"/>
+      <c r="AA8" s="75"/>
+      <c r="AB8" s="75"/>
+      <c r="AC8" s="75"/>
+      <c r="AD8" s="75"/>
+      <c r="AE8" s="75"/>
+      <c r="AF8" s="75"/>
+      <c r="AG8" s="75"/>
+      <c r="AH8" s="75"/>
+      <c r="AI8" s="75"/>
+      <c r="AJ8" s="75"/>
+      <c r="AK8" s="75"/>
+      <c r="AL8" s="75"/>
+      <c r="AM8" s="76"/>
+      <c r="AN8" s="75"/>
+      <c r="AO8" s="75"/>
+      <c r="AP8" s="75"/>
+      <c r="AQ8" s="75"/>
+      <c r="AR8" s="75"/>
+      <c r="AS8" s="75"/>
+      <c r="AT8" s="75"/>
+      <c r="AU8" s="75"/>
+      <c r="AV8" s="75"/>
+      <c r="AW8" s="75"/>
+      <c r="AX8" s="75"/>
+      <c r="AY8" s="75"/>
+      <c r="AZ8" s="75"/>
+      <c r="BA8" s="75"/>
+      <c r="BB8" s="76"/>
+      <c r="BC8" s="75"/>
+      <c r="BD8" s="75"/>
+      <c r="BE8" s="75"/>
+      <c r="BF8" s="75"/>
+      <c r="BG8" s="75"/>
+      <c r="BH8" s="75"/>
+      <c r="BI8" s="75"/>
+      <c r="BJ8" s="75"/>
+      <c r="BK8" s="75"/>
+      <c r="BL8" s="75"/>
+      <c r="BM8" s="75"/>
+      <c r="BN8" s="75"/>
+      <c r="BO8" s="75"/>
+      <c r="BP8" s="75"/>
+      <c r="BQ8" s="75"/>
+      <c r="BR8" s="75"/>
+      <c r="BS8" s="75"/>
+      <c r="BT8" s="75"/>
+      <c r="BU8" s="75"/>
+      <c r="BV8" s="75"/>
+      <c r="BW8" s="75"/>
+      <c r="BX8" s="75"/>
+      <c r="BY8" s="75"/>
+      <c r="BZ8" s="80"/>
     </row>
     <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="75" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="75" t="s">
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="77"/>
-      <c r="S9" s="75" t="s">
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="77"/>
-      <c r="X9" s="75" t="s">
+      <c r="T9" s="78"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="78"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="77"/>
-      <c r="AC9" s="75" t="s">
+      <c r="Y9" s="78"/>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78"/>
+      <c r="AB9" s="79"/>
+      <c r="AC9" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="76"/>
-      <c r="AE9" s="76"/>
-      <c r="AF9" s="76"/>
-      <c r="AG9" s="77"/>
-      <c r="AH9" s="75" t="s">
+      <c r="AD9" s="78"/>
+      <c r="AE9" s="78"/>
+      <c r="AF9" s="78"/>
+      <c r="AG9" s="79"/>
+      <c r="AH9" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="76"/>
-      <c r="AJ9" s="76"/>
-      <c r="AK9" s="76"/>
-      <c r="AL9" s="77"/>
-      <c r="AM9" s="75" t="s">
+      <c r="AI9" s="78"/>
+      <c r="AJ9" s="78"/>
+      <c r="AK9" s="78"/>
+      <c r="AL9" s="79"/>
+      <c r="AM9" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="76"/>
-      <c r="AO9" s="76"/>
-      <c r="AP9" s="76"/>
-      <c r="AQ9" s="77"/>
-      <c r="AR9" s="75" t="s">
+      <c r="AN9" s="78"/>
+      <c r="AO9" s="78"/>
+      <c r="AP9" s="78"/>
+      <c r="AQ9" s="79"/>
+      <c r="AR9" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="76"/>
-      <c r="AT9" s="76"/>
-      <c r="AU9" s="76"/>
-      <c r="AV9" s="77"/>
-      <c r="AW9" s="75" t="s">
+      <c r="AS9" s="78"/>
+      <c r="AT9" s="78"/>
+      <c r="AU9" s="78"/>
+      <c r="AV9" s="79"/>
+      <c r="AW9" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="76"/>
-      <c r="AY9" s="76"/>
-      <c r="AZ9" s="76"/>
-      <c r="BA9" s="77"/>
-      <c r="BB9" s="75" t="s">
+      <c r="AX9" s="78"/>
+      <c r="AY9" s="78"/>
+      <c r="AZ9" s="78"/>
+      <c r="BA9" s="79"/>
+      <c r="BB9" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="76"/>
-      <c r="BD9" s="76"/>
-      <c r="BE9" s="76"/>
-      <c r="BF9" s="77"/>
-      <c r="BG9" s="75" t="s">
+      <c r="BC9" s="78"/>
+      <c r="BD9" s="78"/>
+      <c r="BE9" s="78"/>
+      <c r="BF9" s="79"/>
+      <c r="BG9" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="76"/>
-      <c r="BI9" s="76"/>
-      <c r="BJ9" s="76"/>
-      <c r="BK9" s="77"/>
-      <c r="BL9" s="75" t="s">
+      <c r="BH9" s="78"/>
+      <c r="BI9" s="78"/>
+      <c r="BJ9" s="78"/>
+      <c r="BK9" s="79"/>
+      <c r="BL9" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="76"/>
-      <c r="BN9" s="76"/>
-      <c r="BO9" s="76"/>
-      <c r="BP9" s="77"/>
-      <c r="BQ9" s="75" t="s">
+      <c r="BM9" s="78"/>
+      <c r="BN9" s="78"/>
+      <c r="BO9" s="78"/>
+      <c r="BP9" s="79"/>
+      <c r="BQ9" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="76"/>
-      <c r="BS9" s="76"/>
-      <c r="BT9" s="76"/>
-      <c r="BU9" s="77"/>
-      <c r="BV9" s="75" t="s">
+      <c r="BR9" s="78"/>
+      <c r="BS9" s="78"/>
+      <c r="BT9" s="78"/>
+      <c r="BU9" s="79"/>
+      <c r="BV9" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="76"/>
-      <c r="BX9" s="76"/>
-      <c r="BY9" s="76"/>
-      <c r="BZ9" s="77"/>
+      <c r="BW9" s="78"/>
+      <c r="BX9" s="78"/>
+      <c r="BY9" s="78"/>
+      <c r="BZ9" s="79"/>
     </row>
     <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
@@ -2513,12 +2525,16 @@
       <c r="D16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="37">
+        <v>44851</v>
+      </c>
       <c r="F16" s="37"/>
       <c r="G16" s="38">
         <v>0</v>
       </c>
-      <c r="H16" s="57"/>
+      <c r="H16" s="60">
+        <v>0.75</v>
+      </c>
       <c r="I16" s="44"/>
       <c r="J16" s="45"/>
       <c r="K16" s="46"/>
@@ -2549,11 +2565,21 @@
       <c r="AJ16" s="48"/>
       <c r="AK16" s="48"/>
       <c r="AL16" s="48"/>
-      <c r="AM16" s="48"/>
-      <c r="AN16" s="48"/>
-      <c r="AO16" s="48"/>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="48"/>
+      <c r="AM16" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN16" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO16" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP16" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ16" s="48" t="s">
+        <v>71</v>
+      </c>
       <c r="AR16" s="42"/>
       <c r="AS16" s="42"/>
       <c r="AT16" s="42"/>
@@ -2687,14 +2713,20 @@
       <c r="C18" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="37">
+        <v>44830</v>
+      </c>
       <c r="F18" s="37"/>
       <c r="G18" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="57"/>
+        <v>-44186</v>
+      </c>
+      <c r="H18" s="59">
+        <v>0.5</v>
+      </c>
       <c r="I18" s="44"/>
       <c r="J18" s="45"/>
       <c r="K18" s="46"/>
@@ -2710,14 +2742,30 @@
       <c r="U18" s="40"/>
       <c r="V18" s="40"/>
       <c r="W18" s="40"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="40"/>
-      <c r="Z18" s="40"/>
-      <c r="AA18" s="40"/>
-      <c r="AB18" s="40"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="41"/>
-      <c r="AE18" s="41"/>
+      <c r="X18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB18" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC18" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD18" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE18" s="41" t="s">
+        <v>71</v>
+      </c>
       <c r="AF18" s="41"/>
       <c r="AG18" s="41"/>
       <c r="AH18" s="40"/>
@@ -2774,13 +2822,19 @@
       <c r="C19" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="37">
+        <v>44840</v>
+      </c>
       <c r="F19" s="37"/>
       <c r="G19" s="38">
         <v>0</v>
       </c>
-      <c r="H19" s="57"/>
+      <c r="H19" s="59">
+        <v>0.25</v>
+      </c>
       <c r="I19" s="44"/>
       <c r="J19" s="45"/>
       <c r="K19" s="46"/>
@@ -2804,13 +2858,27 @@
       <c r="AC19" s="41"/>
       <c r="AD19" s="41"/>
       <c r="AE19" s="41"/>
-      <c r="AF19" s="41"/>
-      <c r="AG19" s="41"/>
-      <c r="AH19" s="40"/>
-      <c r="AI19" s="40"/>
-      <c r="AJ19" s="48"/>
-      <c r="AK19" s="48"/>
-      <c r="AL19" s="48"/>
+      <c r="AF19" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG19" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH19" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI19" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ19" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK19" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL19" s="48" t="s">
+        <v>71</v>
+      </c>
       <c r="AM19" s="48"/>
       <c r="AN19" s="48"/>
       <c r="AO19" s="48"/>
@@ -2947,14 +3015,20 @@
       <c r="C21" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="52">
+        <v>44823</v>
+      </c>
       <c r="F21" s="37"/>
       <c r="G21" s="38">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="57"/>
+        <v>-44179</v>
+      </c>
+      <c r="H21" s="59">
+        <v>0.25</v>
+      </c>
       <c r="I21" s="44"/>
       <c r="J21" s="45"/>
       <c r="K21" s="46"/>
@@ -2965,11 +3039,21 @@
       <c r="P21" s="47"/>
       <c r="Q21" s="47"/>
       <c r="R21" s="47"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="40"/>
-      <c r="V21" s="40"/>
-      <c r="W21" s="40"/>
+      <c r="S21" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="T21" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="U21" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="V21" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="W21" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="X21" s="40"/>
       <c r="Y21" s="40"/>
       <c r="Z21" s="40"/>
@@ -4818,15 +4902,25 @@
       <c r="B43" s="51">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
+      <c r="C43" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="52">
+        <v>44823</v>
+      </c>
+      <c r="F43" s="52">
+        <v>44825</v>
+      </c>
       <c r="G43" s="53">
         <f>DAYS360(E43,F43)</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="54"/>
+        <v>2</v>
+      </c>
+      <c r="H43" s="54">
+        <v>1</v>
+      </c>
       <c r="I43" s="44"/>
       <c r="J43" s="45"/>
       <c r="K43" s="46"/>
@@ -4837,8 +4931,12 @@
       <c r="P43" s="49"/>
       <c r="Q43" s="49"/>
       <c r="R43" s="49"/>
-      <c r="S43" s="46"/>
-      <c r="T43" s="46"/>
+      <c r="S43" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="T43" s="46" t="s">
+        <v>71</v>
+      </c>
       <c r="U43" s="46"/>
       <c r="V43" s="46"/>
       <c r="W43" s="46"/>

</xml_diff>

<commit_message>
Work on keypad and screen
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unreal\CPS353-01-Moon-Game\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\MoonGame\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AA40AB-73E7-4555-A264-846E52F5DF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FB4545-C3AA-40CE-932A-C7E7F4040EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7035" yWindow="1567" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -804,6 +804,27 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -818,14 +839,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -835,22 +851,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,22 +1172,22 @@
   </sheetPr>
   <dimension ref="A1:BZ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM34" sqref="AM34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
-    <col min="3" max="3" width="31.73046875" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" customWidth="1"/>
-    <col min="9" max="78" width="3.3984375" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="9" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1267,40 +1267,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
       <c r="AH2" s="12"/>
@@ -1349,7 +1349,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1429,13 +1429,13 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="68"/>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="78" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="70"/>
@@ -1451,7 +1451,7 @@
       <c r="M4" s="68"/>
       <c r="N4" s="68"/>
       <c r="O4" s="68"/>
-      <c r="P4" s="71" t="s">
+      <c r="P4" s="79" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="70"/>
@@ -1517,13 +1517,13 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="67" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="68"/>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="69" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="70"/>
@@ -1539,7 +1539,7 @@
       <c r="M5" s="68"/>
       <c r="N5" s="68"/>
       <c r="O5" s="68"/>
-      <c r="P5" s="82">
+      <c r="P5" s="71">
         <v>44802</v>
       </c>
       <c r="Q5" s="70"/>
@@ -1605,7 +1605,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="23" t="s">
         <v>48</v>
@@ -1687,7 +1687,7 @@
       <c r="BY6" s="22"/>
       <c r="BZ6" s="22"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -1767,209 +1767,209 @@
       <c r="BY7" s="22"/>
       <c r="BZ7" s="22"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="61" t="s">
+      <c r="E8" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="61" t="s">
+      <c r="F8" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="75"/>
-      <c r="V8" s="75"/>
-      <c r="W8" s="75"/>
-      <c r="X8" s="76"/>
-      <c r="Y8" s="75"/>
-      <c r="Z8" s="75"/>
-      <c r="AA8" s="75"/>
-      <c r="AB8" s="75"/>
-      <c r="AC8" s="75"/>
-      <c r="AD8" s="75"/>
-      <c r="AE8" s="75"/>
-      <c r="AF8" s="75"/>
-      <c r="AG8" s="75"/>
-      <c r="AH8" s="75"/>
-      <c r="AI8" s="75"/>
-      <c r="AJ8" s="75"/>
-      <c r="AK8" s="75"/>
-      <c r="AL8" s="75"/>
-      <c r="AM8" s="76"/>
-      <c r="AN8" s="75"/>
-      <c r="AO8" s="75"/>
-      <c r="AP8" s="75"/>
-      <c r="AQ8" s="75"/>
-      <c r="AR8" s="75"/>
-      <c r="AS8" s="75"/>
-      <c r="AT8" s="75"/>
-      <c r="AU8" s="75"/>
-      <c r="AV8" s="75"/>
-      <c r="AW8" s="75"/>
-      <c r="AX8" s="75"/>
-      <c r="AY8" s="75"/>
-      <c r="AZ8" s="75"/>
-      <c r="BA8" s="75"/>
-      <c r="BB8" s="76"/>
-      <c r="BC8" s="75"/>
-      <c r="BD8" s="75"/>
-      <c r="BE8" s="75"/>
-      <c r="BF8" s="75"/>
-      <c r="BG8" s="75"/>
-      <c r="BH8" s="75"/>
-      <c r="BI8" s="75"/>
-      <c r="BJ8" s="75"/>
-      <c r="BK8" s="75"/>
-      <c r="BL8" s="75"/>
-      <c r="BM8" s="75"/>
-      <c r="BN8" s="75"/>
-      <c r="BO8" s="75"/>
-      <c r="BP8" s="75"/>
-      <c r="BQ8" s="75"/>
-      <c r="BR8" s="75"/>
-      <c r="BS8" s="75"/>
-      <c r="BT8" s="75"/>
-      <c r="BU8" s="75"/>
-      <c r="BV8" s="75"/>
-      <c r="BW8" s="75"/>
-      <c r="BX8" s="75"/>
-      <c r="BY8" s="75"/>
-      <c r="BZ8" s="80"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="62"/>
+      <c r="AE8" s="62"/>
+      <c r="AF8" s="62"/>
+      <c r="AG8" s="62"/>
+      <c r="AH8" s="62"/>
+      <c r="AI8" s="62"/>
+      <c r="AJ8" s="62"/>
+      <c r="AK8" s="62"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="61"/>
+      <c r="AN8" s="62"/>
+      <c r="AO8" s="62"/>
+      <c r="AP8" s="62"/>
+      <c r="AQ8" s="62"/>
+      <c r="AR8" s="62"/>
+      <c r="AS8" s="62"/>
+      <c r="AT8" s="62"/>
+      <c r="AU8" s="62"/>
+      <c r="AV8" s="62"/>
+      <c r="AW8" s="62"/>
+      <c r="AX8" s="62"/>
+      <c r="AY8" s="62"/>
+      <c r="AZ8" s="62"/>
+      <c r="BA8" s="62"/>
+      <c r="BB8" s="61"/>
+      <c r="BC8" s="62"/>
+      <c r="BD8" s="62"/>
+      <c r="BE8" s="62"/>
+      <c r="BF8" s="62"/>
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62"/>
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62"/>
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+      <c r="BM8" s="62"/>
+      <c r="BN8" s="62"/>
+      <c r="BO8" s="62"/>
+      <c r="BP8" s="62"/>
+      <c r="BQ8" s="62"/>
+      <c r="BR8" s="62"/>
+      <c r="BS8" s="62"/>
+      <c r="BT8" s="62"/>
+      <c r="BU8" s="62"/>
+      <c r="BV8" s="62"/>
+      <c r="BW8" s="62"/>
+      <c r="BX8" s="62"/>
+      <c r="BY8" s="62"/>
+      <c r="BZ8" s="63"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="77" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="77" t="s">
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="79"/>
-      <c r="S9" s="77" t="s">
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="79"/>
-      <c r="X9" s="77" t="s">
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="79"/>
-      <c r="AC9" s="77" t="s">
+      <c r="Y9" s="65"/>
+      <c r="Z9" s="65"/>
+      <c r="AA9" s="65"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="79"/>
-      <c r="AH9" s="77" t="s">
+      <c r="AD9" s="65"/>
+      <c r="AE9" s="65"/>
+      <c r="AF9" s="65"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="78"/>
-      <c r="AL9" s="79"/>
-      <c r="AM9" s="77" t="s">
+      <c r="AI9" s="65"/>
+      <c r="AJ9" s="65"/>
+      <c r="AK9" s="65"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78"/>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="79"/>
-      <c r="AR9" s="77" t="s">
+      <c r="AN9" s="65"/>
+      <c r="AO9" s="65"/>
+      <c r="AP9" s="65"/>
+      <c r="AQ9" s="66"/>
+      <c r="AR9" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="78"/>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78"/>
-      <c r="AV9" s="79"/>
-      <c r="AW9" s="77" t="s">
+      <c r="AS9" s="65"/>
+      <c r="AT9" s="65"/>
+      <c r="AU9" s="65"/>
+      <c r="AV9" s="66"/>
+      <c r="AW9" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78"/>
-      <c r="AZ9" s="78"/>
-      <c r="BA9" s="79"/>
-      <c r="BB9" s="77" t="s">
+      <c r="AX9" s="65"/>
+      <c r="AY9" s="65"/>
+      <c r="AZ9" s="65"/>
+      <c r="BA9" s="66"/>
+      <c r="BB9" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="78"/>
-      <c r="BD9" s="78"/>
-      <c r="BE9" s="78"/>
-      <c r="BF9" s="79"/>
-      <c r="BG9" s="77" t="s">
+      <c r="BC9" s="65"/>
+      <c r="BD9" s="65"/>
+      <c r="BE9" s="65"/>
+      <c r="BF9" s="66"/>
+      <c r="BG9" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="78"/>
-      <c r="BI9" s="78"/>
-      <c r="BJ9" s="78"/>
-      <c r="BK9" s="79"/>
-      <c r="BL9" s="77" t="s">
+      <c r="BH9" s="65"/>
+      <c r="BI9" s="65"/>
+      <c r="BJ9" s="65"/>
+      <c r="BK9" s="66"/>
+      <c r="BL9" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="78"/>
-      <c r="BN9" s="78"/>
-      <c r="BO9" s="78"/>
-      <c r="BP9" s="79"/>
-      <c r="BQ9" s="77" t="s">
+      <c r="BM9" s="65"/>
+      <c r="BN9" s="65"/>
+      <c r="BO9" s="65"/>
+      <c r="BP9" s="66"/>
+      <c r="BQ9" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="78"/>
-      <c r="BS9" s="78"/>
-      <c r="BT9" s="78"/>
-      <c r="BU9" s="79"/>
-      <c r="BV9" s="77" t="s">
+      <c r="BR9" s="65"/>
+      <c r="BS9" s="65"/>
+      <c r="BT9" s="65"/>
+      <c r="BU9" s="66"/>
+      <c r="BV9" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="78"/>
-      <c r="BX9" s="78"/>
-      <c r="BY9" s="78"/>
-      <c r="BZ9" s="79"/>
+      <c r="BW9" s="65"/>
+      <c r="BX9" s="65"/>
+      <c r="BY9" s="65"/>
+      <c r="BZ9" s="66"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="27">
         <v>1</v>
@@ -2053,7 +2053,7 @@
       <c r="BY10" s="33"/>
       <c r="BZ10" s="33"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
       <c r="B11" s="35">
         <v>1.1000000000000001</v>
@@ -2148,7 +2148,7 @@
       <c r="BY11" s="40"/>
       <c r="BZ11" s="40"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34"/>
       <c r="B12" s="35" t="s">
         <v>13</v>
@@ -2243,7 +2243,7 @@
       <c r="BY12" s="40"/>
       <c r="BZ12" s="40"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34"/>
       <c r="B13" s="35">
         <v>1.2</v>
@@ -2338,7 +2338,7 @@
       <c r="BY13" s="40"/>
       <c r="BZ13" s="40"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34"/>
       <c r="B14" s="35">
         <v>1.3</v>
@@ -2433,7 +2433,7 @@
       <c r="BY14" s="40"/>
       <c r="BZ14" s="40"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
       <c r="B15" s="27">
         <v>2</v>
@@ -2517,7 +2517,7 @@
       <c r="BY15" s="33"/>
       <c r="BZ15" s="33"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34"/>
       <c r="B16" s="35">
         <v>2.1</v>
@@ -2619,7 +2619,7 @@
       <c r="BY16" s="40"/>
       <c r="BZ16" s="40"/>
     </row>
-    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="34"/>
       <c r="B17" s="35">
         <v>2.2000000000000002</v>
@@ -2708,7 +2708,7 @@
       <c r="BY17" s="40"/>
       <c r="BZ17" s="40"/>
     </row>
-    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
       <c r="B18" s="35">
         <v>2.2999999999999998</v>
@@ -2817,7 +2817,7 @@
       <c r="BY18" s="40"/>
       <c r="BZ18" s="40"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="34"/>
       <c r="B19" s="35" t="s">
         <v>15</v>
@@ -2923,7 +2923,7 @@
       <c r="BY19" s="40"/>
       <c r="BZ19" s="40"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="34"/>
       <c r="B20" s="35">
         <v>2.4</v>
@@ -3010,7 +3010,7 @@
       <c r="BY20" s="40"/>
       <c r="BZ20" s="40"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="34"/>
       <c r="B21" s="35">
         <v>2.5</v>
@@ -3113,7 +3113,7 @@
       <c r="BY21" s="40"/>
       <c r="BZ21" s="40"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
       <c r="B22" s="35">
         <v>2.6</v>
@@ -3201,7 +3201,7 @@
       <c r="BY22" s="40"/>
       <c r="BZ22" s="40"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="34"/>
       <c r="B23" s="35">
         <v>2.7</v>
@@ -3288,7 +3288,7 @@
       <c r="BY23" s="40"/>
       <c r="BZ23" s="40"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="34"/>
       <c r="B24" s="35">
         <v>2.8</v>
@@ -3373,7 +3373,7 @@
       <c r="BY24" s="40"/>
       <c r="BZ24" s="40"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34"/>
       <c r="B25" s="35">
         <v>2.9</v>
@@ -3457,7 +3457,7 @@
       <c r="BY25" s="40"/>
       <c r="BZ25" s="40"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
       <c r="B26" s="50">
         <v>2.1</v>
@@ -3542,7 +3542,7 @@
       <c r="BY26" s="40"/>
       <c r="BZ26" s="40"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="50">
         <v>2.11</v>
@@ -3626,7 +3626,7 @@
       <c r="BY27" s="40"/>
       <c r="BZ27" s="40"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="27">
         <v>3</v>
@@ -3710,7 +3710,7 @@
       <c r="BY28" s="33"/>
       <c r="BZ28" s="33"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
       <c r="B29" s="35">
         <v>3.1</v>
@@ -3799,7 +3799,7 @@
       <c r="BY29" s="40"/>
       <c r="BZ29" s="40"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="35">
         <v>3.2</v>
@@ -3887,7 +3887,7 @@
       <c r="BY30" s="40"/>
       <c r="BZ30" s="40"/>
     </row>
-    <row r="31" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
       <c r="B31" s="35" t="s">
         <v>17</v>
@@ -3976,7 +3976,7 @@
       <c r="BY31" s="40"/>
       <c r="BZ31" s="40"/>
     </row>
-    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="35" t="s">
         <v>18</v>
@@ -4065,7 +4065,7 @@
       <c r="BY32" s="40"/>
       <c r="BZ32" s="40"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="35">
         <v>3.3</v>
@@ -4154,7 +4154,7 @@
       <c r="BY33" s="40"/>
       <c r="BZ33" s="40"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="51" t="s">
         <v>19</v>
@@ -4244,7 +4244,7 @@
       <c r="BY34" s="46"/>
       <c r="BZ34" s="46"/>
     </row>
-    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="51"/>
       <c r="C35" s="57" t="s">
@@ -4290,11 +4290,17 @@
       <c r="AM35" s="46"/>
       <c r="AN35" s="46"/>
       <c r="AO35" s="46"/>
-      <c r="AP35" s="46"/>
+      <c r="AP35" s="46" t="s">
+        <v>71</v>
+      </c>
       <c r="AQ35" s="46"/>
       <c r="AR35" s="42"/>
-      <c r="AS35" s="42"/>
-      <c r="AT35" s="42"/>
+      <c r="AS35" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT35" s="42" t="s">
+        <v>71</v>
+      </c>
       <c r="AU35" s="42"/>
       <c r="AV35" s="42"/>
       <c r="AW35" s="46"/>
@@ -4328,7 +4334,7 @@
       <c r="BY35" s="46"/>
       <c r="BZ35" s="46"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="51"/>
       <c r="C36" s="57" t="s">
@@ -4418,7 +4424,7 @@
       <c r="BY36" s="46"/>
       <c r="BZ36" s="46"/>
     </row>
-    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="51"/>
       <c r="C37" s="57" t="s">
@@ -4435,7 +4441,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="54">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="I37" s="44"/>
       <c r="J37" s="45"/>
@@ -4475,8 +4481,12 @@
       </c>
       <c r="AQ37" s="46"/>
       <c r="AR37" s="42"/>
-      <c r="AS37" s="42"/>
-      <c r="AT37" s="42"/>
+      <c r="AS37" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT37" s="42" t="s">
+        <v>71</v>
+      </c>
       <c r="AU37" s="42"/>
       <c r="AV37" s="42"/>
       <c r="AW37" s="46"/>
@@ -4510,7 +4520,7 @@
       <c r="BY37" s="46"/>
       <c r="BZ37" s="46"/>
     </row>
-    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="51"/>
       <c r="C38" s="57"/>
       <c r="D38" s="36"/>
@@ -4591,7 +4601,7 @@
       <c r="BY38" s="46"/>
       <c r="BZ38" s="46"/>
     </row>
-    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="51"/>
       <c r="C39" s="57"/>
       <c r="D39" s="36"/>
@@ -4672,7 +4682,7 @@
       <c r="BY39" s="46"/>
       <c r="BZ39" s="46"/>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="51"/>
       <c r="C40" s="57"/>
       <c r="D40" s="36"/>
@@ -4753,7 +4763,7 @@
       <c r="BY40" s="46"/>
       <c r="BZ40" s="46"/>
     </row>
-    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="51"/>
       <c r="C41" s="57"/>
       <c r="D41" s="36"/>
@@ -4834,7 +4844,7 @@
       <c r="BY41" s="46"/>
       <c r="BZ41" s="46"/>
     </row>
-    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="27">
         <v>4</v>
       </c>
@@ -4917,7 +4927,7 @@
       <c r="BY42" s="33"/>
       <c r="BZ42" s="33"/>
     </row>
-    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="51">
         <v>4.0999999999999996</v>
       </c>
@@ -5015,7 +5025,7 @@
       <c r="BY43" s="46"/>
       <c r="BZ43" s="46"/>
     </row>
-    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="51">
         <v>4.2</v>
       </c>
@@ -5098,7 +5108,7 @@
       <c r="BY44" s="46"/>
       <c r="BZ44" s="46"/>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="51" t="s">
         <v>42</v>
       </c>
@@ -5182,7 +5192,7 @@
       <c r="BY45" s="46"/>
       <c r="BZ45" s="46"/>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="51" t="s">
         <v>43</v>
       </c>
@@ -5266,7 +5276,7 @@
       <c r="BY46" s="46"/>
       <c r="BZ46" s="46"/>
     </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="51">
         <v>4.3</v>
       </c>
@@ -5350,7 +5360,7 @@
       <c r="BY47" s="46"/>
       <c r="BZ47" s="46"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="51" t="s">
         <v>44</v>
       </c>
@@ -5435,6 +5445,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5451,26 +5481,6 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H48">
     <cfRule type="colorScale" priority="6">
@@ -5498,9 +5508,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5733,27 +5746,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5778,9 +5779,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Progress on Inventory System
Player can somewhat spawn items and destroy them on inventory select
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF10B15-948C-4A24-B949-B38204662354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD02BF-B76F-447D-A7D6-55279ED2AD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>JV</t>
+  </si>
+  <si>
+    <t>Trash Bins</t>
   </si>
 </sst>
 </file>
@@ -776,6 +779,27 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,14 +814,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -807,22 +826,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,7 +1148,7 @@
   <dimension ref="A1:BZ48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1241,38 +1244,38 @@
     </row>
     <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1407,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="58"/>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="68" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="60"/>
@@ -1423,7 +1426,7 @@
       <c r="M4" s="58"/>
       <c r="N4" s="58"/>
       <c r="O4" s="58"/>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="69" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="60"/>
@@ -1495,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="58"/>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="59" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="60"/>
@@ -1511,7 +1514,7 @@
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
       <c r="O5" s="58"/>
-      <c r="P5" s="72">
+      <c r="P5" s="61">
         <v>44802</v>
       </c>
       <c r="Q5" s="60"/>
@@ -1741,205 +1744,205 @@
     </row>
     <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="62" t="s">
+      <c r="H8" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
-      <c r="U8" s="65"/>
-      <c r="V8" s="65"/>
-      <c r="W8" s="65"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="65"/>
-      <c r="Z8" s="65"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
-      <c r="AC8" s="65"/>
-      <c r="AD8" s="65"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="65"/>
-      <c r="AG8" s="65"/>
-      <c r="AH8" s="65"/>
-      <c r="AI8" s="65"/>
-      <c r="AJ8" s="65"/>
-      <c r="AK8" s="65"/>
-      <c r="AL8" s="65"/>
-      <c r="AM8" s="66"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="65"/>
-      <c r="AP8" s="65"/>
-      <c r="AQ8" s="65"/>
-      <c r="AR8" s="65"/>
-      <c r="AS8" s="65"/>
-      <c r="AT8" s="65"/>
-      <c r="AU8" s="65"/>
-      <c r="AV8" s="65"/>
-      <c r="AW8" s="65"/>
-      <c r="AX8" s="65"/>
-      <c r="AY8" s="65"/>
-      <c r="AZ8" s="65"/>
-      <c r="BA8" s="65"/>
-      <c r="BB8" s="66"/>
-      <c r="BC8" s="65"/>
-      <c r="BD8" s="65"/>
-      <c r="BE8" s="65"/>
-      <c r="BF8" s="65"/>
-      <c r="BG8" s="65"/>
-      <c r="BH8" s="65"/>
-      <c r="BI8" s="65"/>
-      <c r="BJ8" s="65"/>
-      <c r="BK8" s="65"/>
-      <c r="BL8" s="65"/>
-      <c r="BM8" s="65"/>
-      <c r="BN8" s="65"/>
-      <c r="BO8" s="65"/>
-      <c r="BP8" s="65"/>
-      <c r="BQ8" s="65"/>
-      <c r="BR8" s="65"/>
-      <c r="BS8" s="65"/>
-      <c r="BT8" s="65"/>
-      <c r="BU8" s="65"/>
-      <c r="BV8" s="65"/>
-      <c r="BW8" s="65"/>
-      <c r="BX8" s="65"/>
-      <c r="BY8" s="65"/>
-      <c r="BZ8" s="70"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
+      <c r="AC8" s="52"/>
+      <c r="AD8" s="52"/>
+      <c r="AE8" s="52"/>
+      <c r="AF8" s="52"/>
+      <c r="AG8" s="52"/>
+      <c r="AH8" s="52"/>
+      <c r="AI8" s="52"/>
+      <c r="AJ8" s="52"/>
+      <c r="AK8" s="52"/>
+      <c r="AL8" s="52"/>
+      <c r="AM8" s="51"/>
+      <c r="AN8" s="52"/>
+      <c r="AO8" s="52"/>
+      <c r="AP8" s="52"/>
+      <c r="AQ8" s="52"/>
+      <c r="AR8" s="52"/>
+      <c r="AS8" s="52"/>
+      <c r="AT8" s="52"/>
+      <c r="AU8" s="52"/>
+      <c r="AV8" s="52"/>
+      <c r="AW8" s="52"/>
+      <c r="AX8" s="52"/>
+      <c r="AY8" s="52"/>
+      <c r="AZ8" s="52"/>
+      <c r="BA8" s="52"/>
+      <c r="BB8" s="51"/>
+      <c r="BC8" s="52"/>
+      <c r="BD8" s="52"/>
+      <c r="BE8" s="52"/>
+      <c r="BF8" s="52"/>
+      <c r="BG8" s="52"/>
+      <c r="BH8" s="52"/>
+      <c r="BI8" s="52"/>
+      <c r="BJ8" s="52"/>
+      <c r="BK8" s="52"/>
+      <c r="BL8" s="52"/>
+      <c r="BM8" s="52"/>
+      <c r="BN8" s="52"/>
+      <c r="BO8" s="52"/>
+      <c r="BP8" s="52"/>
+      <c r="BQ8" s="52"/>
+      <c r="BR8" s="52"/>
+      <c r="BS8" s="52"/>
+      <c r="BT8" s="52"/>
+      <c r="BU8" s="52"/>
+      <c r="BV8" s="52"/>
+      <c r="BW8" s="52"/>
+      <c r="BX8" s="52"/>
+      <c r="BY8" s="52"/>
+      <c r="BZ8" s="53"/>
     </row>
     <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="67" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="67" t="s">
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="67" t="s">
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="68"/>
-      <c r="U9" s="68"/>
-      <c r="V9" s="68"/>
-      <c r="W9" s="69"/>
-      <c r="X9" s="67" t="s">
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="68"/>
-      <c r="Z9" s="68"/>
-      <c r="AA9" s="68"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="67" t="s">
+      <c r="Y9" s="55"/>
+      <c r="Z9" s="55"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="68"/>
-      <c r="AE9" s="68"/>
-      <c r="AF9" s="68"/>
-      <c r="AG9" s="69"/>
-      <c r="AH9" s="67" t="s">
+      <c r="AD9" s="55"/>
+      <c r="AE9" s="55"/>
+      <c r="AF9" s="55"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="68"/>
-      <c r="AJ9" s="68"/>
-      <c r="AK9" s="68"/>
-      <c r="AL9" s="69"/>
-      <c r="AM9" s="67" t="s">
+      <c r="AI9" s="55"/>
+      <c r="AJ9" s="55"/>
+      <c r="AK9" s="55"/>
+      <c r="AL9" s="56"/>
+      <c r="AM9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="68"/>
-      <c r="AO9" s="68"/>
-      <c r="AP9" s="68"/>
-      <c r="AQ9" s="69"/>
-      <c r="AR9" s="67" t="s">
+      <c r="AN9" s="55"/>
+      <c r="AO9" s="55"/>
+      <c r="AP9" s="55"/>
+      <c r="AQ9" s="56"/>
+      <c r="AR9" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="68"/>
-      <c r="AT9" s="68"/>
-      <c r="AU9" s="68"/>
-      <c r="AV9" s="69"/>
-      <c r="AW9" s="67" t="s">
+      <c r="AS9" s="55"/>
+      <c r="AT9" s="55"/>
+      <c r="AU9" s="55"/>
+      <c r="AV9" s="56"/>
+      <c r="AW9" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="68"/>
-      <c r="AY9" s="68"/>
-      <c r="AZ9" s="68"/>
-      <c r="BA9" s="69"/>
-      <c r="BB9" s="67" t="s">
+      <c r="AX9" s="55"/>
+      <c r="AY9" s="55"/>
+      <c r="AZ9" s="55"/>
+      <c r="BA9" s="56"/>
+      <c r="BB9" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="68"/>
-      <c r="BD9" s="68"/>
-      <c r="BE9" s="68"/>
-      <c r="BF9" s="69"/>
-      <c r="BG9" s="67" t="s">
+      <c r="BC9" s="55"/>
+      <c r="BD9" s="55"/>
+      <c r="BE9" s="55"/>
+      <c r="BF9" s="56"/>
+      <c r="BG9" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="68"/>
-      <c r="BI9" s="68"/>
-      <c r="BJ9" s="68"/>
-      <c r="BK9" s="69"/>
-      <c r="BL9" s="67" t="s">
+      <c r="BH9" s="55"/>
+      <c r="BI9" s="55"/>
+      <c r="BJ9" s="55"/>
+      <c r="BK9" s="56"/>
+      <c r="BL9" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="68"/>
-      <c r="BN9" s="68"/>
-      <c r="BO9" s="68"/>
-      <c r="BP9" s="69"/>
-      <c r="BQ9" s="67" t="s">
+      <c r="BM9" s="55"/>
+      <c r="BN9" s="55"/>
+      <c r="BO9" s="55"/>
+      <c r="BP9" s="56"/>
+      <c r="BQ9" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="68"/>
-      <c r="BS9" s="68"/>
-      <c r="BT9" s="68"/>
-      <c r="BU9" s="69"/>
-      <c r="BV9" s="67" t="s">
+      <c r="BR9" s="55"/>
+      <c r="BS9" s="55"/>
+      <c r="BT9" s="55"/>
+      <c r="BU9" s="56"/>
+      <c r="BV9" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="68"/>
-      <c r="BX9" s="68"/>
-      <c r="BY9" s="68"/>
-      <c r="BZ9" s="69"/>
+      <c r="BW9" s="55"/>
+      <c r="BX9" s="55"/>
+      <c r="BY9" s="55"/>
+      <c r="BZ9" s="56"/>
     </row>
     <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -3879,7 +3882,7 @@
         <v>-44206</v>
       </c>
       <c r="H31" s="37">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="I31" s="42"/>
       <c r="J31" s="43"/>
@@ -4234,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="37">
-        <v>0.03</v>
+        <v>0.75</v>
       </c>
       <c r="I35" s="42"/>
       <c r="J35" s="43"/>
@@ -4501,14 +4504,18 @@
     </row>
     <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
-      <c r="C38" s="47"/>
+      <c r="C38" s="47" t="s">
+        <v>74</v>
+      </c>
       <c r="D38" s="34"/>
       <c r="E38" s="35"/>
       <c r="F38" s="35"/>
       <c r="G38" s="36">
         <v>0</v>
       </c>
-      <c r="H38" s="37"/>
+      <c r="H38" s="37">
+        <v>0.8</v>
+      </c>
       <c r="I38" s="42"/>
       <c r="J38" s="43"/>
       <c r="K38" s="38"/>
@@ -5423,6 +5430,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5439,26 +5466,6 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H48">
     <cfRule type="colorScale" priority="6">
@@ -5486,9 +5493,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5721,27 +5731,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5766,9 +5764,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More Inventory System Progress
Items will now appear and disappear when you select/deselect a slot. Waiting on line trace function to implement "holding" state
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD02BF-B76F-447D-A7D6-55279ED2AD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1738B994-F163-4FD6-ABE7-59EF74FFD92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,27 +779,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -814,9 +793,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -826,6 +810,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:BZ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1244,38 +1244,38 @@
     </row>
     <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="58"/>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="59" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="60"/>
@@ -1426,7 +1426,7 @@
       <c r="M4" s="58"/>
       <c r="N4" s="58"/>
       <c r="O4" s="58"/>
-      <c r="P4" s="69" t="s">
+      <c r="P4" s="61" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="60"/>
@@ -1498,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="58"/>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="71" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="60"/>
@@ -1514,7 +1514,7 @@
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
       <c r="O5" s="58"/>
-      <c r="P5" s="61">
+      <c r="P5" s="72">
         <v>44802</v>
       </c>
       <c r="Q5" s="60"/>
@@ -1744,205 +1744,205 @@
     </row>
     <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="52"/>
-      <c r="AE8" s="52"/>
-      <c r="AF8" s="52"/>
-      <c r="AG8" s="52"/>
-      <c r="AH8" s="52"/>
-      <c r="AI8" s="52"/>
-      <c r="AJ8" s="52"/>
-      <c r="AK8" s="52"/>
-      <c r="AL8" s="52"/>
-      <c r="AM8" s="51"/>
-      <c r="AN8" s="52"/>
-      <c r="AO8" s="52"/>
-      <c r="AP8" s="52"/>
-      <c r="AQ8" s="52"/>
-      <c r="AR8" s="52"/>
-      <c r="AS8" s="52"/>
-      <c r="AT8" s="52"/>
-      <c r="AU8" s="52"/>
-      <c r="AV8" s="52"/>
-      <c r="AW8" s="52"/>
-      <c r="AX8" s="52"/>
-      <c r="AY8" s="52"/>
-      <c r="AZ8" s="52"/>
-      <c r="BA8" s="52"/>
-      <c r="BB8" s="51"/>
-      <c r="BC8" s="52"/>
-      <c r="BD8" s="52"/>
-      <c r="BE8" s="52"/>
-      <c r="BF8" s="52"/>
-      <c r="BG8" s="52"/>
-      <c r="BH8" s="52"/>
-      <c r="BI8" s="52"/>
-      <c r="BJ8" s="52"/>
-      <c r="BK8" s="52"/>
-      <c r="BL8" s="52"/>
-      <c r="BM8" s="52"/>
-      <c r="BN8" s="52"/>
-      <c r="BO8" s="52"/>
-      <c r="BP8" s="52"/>
-      <c r="BQ8" s="52"/>
-      <c r="BR8" s="52"/>
-      <c r="BS8" s="52"/>
-      <c r="BT8" s="52"/>
-      <c r="BU8" s="52"/>
-      <c r="BV8" s="52"/>
-      <c r="BW8" s="52"/>
-      <c r="BX8" s="52"/>
-      <c r="BY8" s="52"/>
-      <c r="BZ8" s="53"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="65"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AI8" s="65"/>
+      <c r="AJ8" s="65"/>
+      <c r="AK8" s="65"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="66"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
+      <c r="AP8" s="65"/>
+      <c r="AQ8" s="65"/>
+      <c r="AR8" s="65"/>
+      <c r="AS8" s="65"/>
+      <c r="AT8" s="65"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
+      <c r="AW8" s="65"/>
+      <c r="AX8" s="65"/>
+      <c r="AY8" s="65"/>
+      <c r="AZ8" s="65"/>
+      <c r="BA8" s="65"/>
+      <c r="BB8" s="66"/>
+      <c r="BC8" s="65"/>
+      <c r="BD8" s="65"/>
+      <c r="BE8" s="65"/>
+      <c r="BF8" s="65"/>
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65"/>
+      <c r="BL8" s="65"/>
+      <c r="BM8" s="65"/>
+      <c r="BN8" s="65"/>
+      <c r="BO8" s="65"/>
+      <c r="BP8" s="65"/>
+      <c r="BQ8" s="65"/>
+      <c r="BR8" s="65"/>
+      <c r="BS8" s="65"/>
+      <c r="BT8" s="65"/>
+      <c r="BU8" s="65"/>
+      <c r="BV8" s="65"/>
+      <c r="BW8" s="65"/>
+      <c r="BX8" s="65"/>
+      <c r="BY8" s="65"/>
+      <c r="BZ8" s="70"/>
     </row>
     <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="54" t="s">
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="54" t="s">
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="54" t="s">
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="54" t="s">
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="56"/>
-      <c r="AC9" s="54" t="s">
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="55"/>
-      <c r="AE9" s="55"/>
-      <c r="AF9" s="55"/>
-      <c r="AG9" s="56"/>
-      <c r="AH9" s="54" t="s">
+      <c r="AD9" s="68"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="69"/>
+      <c r="AH9" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="55"/>
-      <c r="AJ9" s="55"/>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="56"/>
-      <c r="AM9" s="54" t="s">
+      <c r="AI9" s="68"/>
+      <c r="AJ9" s="68"/>
+      <c r="AK9" s="68"/>
+      <c r="AL9" s="69"/>
+      <c r="AM9" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="56"/>
-      <c r="AR9" s="54" t="s">
+      <c r="AN9" s="68"/>
+      <c r="AO9" s="68"/>
+      <c r="AP9" s="68"/>
+      <c r="AQ9" s="69"/>
+      <c r="AR9" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
-      <c r="AU9" s="55"/>
-      <c r="AV9" s="56"/>
-      <c r="AW9" s="54" t="s">
+      <c r="AS9" s="68"/>
+      <c r="AT9" s="68"/>
+      <c r="AU9" s="68"/>
+      <c r="AV9" s="69"/>
+      <c r="AW9" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="55"/>
-      <c r="AY9" s="55"/>
-      <c r="AZ9" s="55"/>
-      <c r="BA9" s="56"/>
-      <c r="BB9" s="54" t="s">
+      <c r="AX9" s="68"/>
+      <c r="AY9" s="68"/>
+      <c r="AZ9" s="68"/>
+      <c r="BA9" s="69"/>
+      <c r="BB9" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="55"/>
-      <c r="BD9" s="55"/>
-      <c r="BE9" s="55"/>
-      <c r="BF9" s="56"/>
-      <c r="BG9" s="54" t="s">
+      <c r="BC9" s="68"/>
+      <c r="BD9" s="68"/>
+      <c r="BE9" s="68"/>
+      <c r="BF9" s="69"/>
+      <c r="BG9" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="55"/>
-      <c r="BI9" s="55"/>
-      <c r="BJ9" s="55"/>
-      <c r="BK9" s="56"/>
-      <c r="BL9" s="54" t="s">
+      <c r="BH9" s="68"/>
+      <c r="BI9" s="68"/>
+      <c r="BJ9" s="68"/>
+      <c r="BK9" s="69"/>
+      <c r="BL9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="55"/>
-      <c r="BN9" s="55"/>
-      <c r="BO9" s="55"/>
-      <c r="BP9" s="56"/>
-      <c r="BQ9" s="54" t="s">
+      <c r="BM9" s="68"/>
+      <c r="BN9" s="68"/>
+      <c r="BO9" s="68"/>
+      <c r="BP9" s="69"/>
+      <c r="BQ9" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="55"/>
-      <c r="BS9" s="55"/>
-      <c r="BT9" s="55"/>
-      <c r="BU9" s="56"/>
-      <c r="BV9" s="54" t="s">
+      <c r="BR9" s="68"/>
+      <c r="BS9" s="68"/>
+      <c r="BT9" s="68"/>
+      <c r="BU9" s="69"/>
+      <c r="BV9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="55"/>
-      <c r="BX9" s="55"/>
-      <c r="BY9" s="55"/>
-      <c r="BZ9" s="56"/>
+      <c r="BW9" s="68"/>
+      <c r="BX9" s="68"/>
+      <c r="BY9" s="68"/>
+      <c r="BZ9" s="69"/>
     </row>
     <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
@@ -3882,7 +3882,7 @@
         <v>-44206</v>
       </c>
       <c r="H31" s="37">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I31" s="42"/>
       <c r="J31" s="43"/>
@@ -5430,26 +5430,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5466,6 +5446,26 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H48">
     <cfRule type="colorScale" priority="6">
@@ -5493,12 +5493,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5731,15 +5728,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5764,18 +5773,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gahnt Chart update, flowchart added for light puzzle
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UE_4.27\MoonGame\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4B3138-3CCB-4A8F-B130-065004C7B072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2D90D-19B5-4AAE-B4A5-1EE279EF7E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>LR, BJ</t>
+  </si>
+  <si>
+    <t>Light puzzle</t>
+  </si>
+  <si>
+    <t>Moving Light puzzle</t>
   </si>
 </sst>
 </file>
@@ -788,27 +794,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -823,9 +808,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -835,6 +825,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1156,22 +1162,22 @@
   </sheetPr>
   <dimension ref="A1:BZ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" customWidth="1"/>
-    <col min="9" max="78" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="9" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1251,40 +1257,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1333,7 +1339,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1413,13 +1419,13 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="58"/>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="59" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="60"/>
@@ -1435,7 +1441,7 @@
       <c r="M4" s="58"/>
       <c r="N4" s="58"/>
       <c r="O4" s="58"/>
-      <c r="P4" s="69" t="s">
+      <c r="P4" s="61" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="60"/>
@@ -1501,13 +1507,13 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="58"/>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="71" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="60"/>
@@ -1523,7 +1529,7 @@
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
       <c r="O5" s="58"/>
-      <c r="P5" s="61">
+      <c r="P5" s="72">
         <v>44802</v>
       </c>
       <c r="Q5" s="60"/>
@@ -1589,7 +1595,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
         <v>48</v>
@@ -1671,7 +1677,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1751,209 +1757,209 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="52"/>
-      <c r="AE8" s="52"/>
-      <c r="AF8" s="52"/>
-      <c r="AG8" s="52"/>
-      <c r="AH8" s="52"/>
-      <c r="AI8" s="52"/>
-      <c r="AJ8" s="52"/>
-      <c r="AK8" s="52"/>
-      <c r="AL8" s="52"/>
-      <c r="AM8" s="51"/>
-      <c r="AN8" s="52"/>
-      <c r="AO8" s="52"/>
-      <c r="AP8" s="52"/>
-      <c r="AQ8" s="52"/>
-      <c r="AR8" s="52"/>
-      <c r="AS8" s="52"/>
-      <c r="AT8" s="52"/>
-      <c r="AU8" s="52"/>
-      <c r="AV8" s="52"/>
-      <c r="AW8" s="52"/>
-      <c r="AX8" s="52"/>
-      <c r="AY8" s="52"/>
-      <c r="AZ8" s="52"/>
-      <c r="BA8" s="52"/>
-      <c r="BB8" s="51"/>
-      <c r="BC8" s="52"/>
-      <c r="BD8" s="52"/>
-      <c r="BE8" s="52"/>
-      <c r="BF8" s="52"/>
-      <c r="BG8" s="52"/>
-      <c r="BH8" s="52"/>
-      <c r="BI8" s="52"/>
-      <c r="BJ8" s="52"/>
-      <c r="BK8" s="52"/>
-      <c r="BL8" s="52"/>
-      <c r="BM8" s="52"/>
-      <c r="BN8" s="52"/>
-      <c r="BO8" s="52"/>
-      <c r="BP8" s="52"/>
-      <c r="BQ8" s="52"/>
-      <c r="BR8" s="52"/>
-      <c r="BS8" s="52"/>
-      <c r="BT8" s="52"/>
-      <c r="BU8" s="52"/>
-      <c r="BV8" s="52"/>
-      <c r="BW8" s="52"/>
-      <c r="BX8" s="52"/>
-      <c r="BY8" s="52"/>
-      <c r="BZ8" s="53"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="65"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="65"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AI8" s="65"/>
+      <c r="AJ8" s="65"/>
+      <c r="AK8" s="65"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="66"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
+      <c r="AP8" s="65"/>
+      <c r="AQ8" s="65"/>
+      <c r="AR8" s="65"/>
+      <c r="AS8" s="65"/>
+      <c r="AT8" s="65"/>
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
+      <c r="AW8" s="65"/>
+      <c r="AX8" s="65"/>
+      <c r="AY8" s="65"/>
+      <c r="AZ8" s="65"/>
+      <c r="BA8" s="65"/>
+      <c r="BB8" s="66"/>
+      <c r="BC8" s="65"/>
+      <c r="BD8" s="65"/>
+      <c r="BE8" s="65"/>
+      <c r="BF8" s="65"/>
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65"/>
+      <c r="BL8" s="65"/>
+      <c r="BM8" s="65"/>
+      <c r="BN8" s="65"/>
+      <c r="BO8" s="65"/>
+      <c r="BP8" s="65"/>
+      <c r="BQ8" s="65"/>
+      <c r="BR8" s="65"/>
+      <c r="BS8" s="65"/>
+      <c r="BT8" s="65"/>
+      <c r="BU8" s="65"/>
+      <c r="BV8" s="65"/>
+      <c r="BW8" s="65"/>
+      <c r="BX8" s="65"/>
+      <c r="BY8" s="65"/>
+      <c r="BZ8" s="70"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="54" t="s">
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="54" t="s">
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="54" t="s">
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="54" t="s">
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="56"/>
-      <c r="AC9" s="54" t="s">
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="55"/>
-      <c r="AE9" s="55"/>
-      <c r="AF9" s="55"/>
-      <c r="AG9" s="56"/>
-      <c r="AH9" s="54" t="s">
+      <c r="AD9" s="68"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="69"/>
+      <c r="AH9" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="55"/>
-      <c r="AJ9" s="55"/>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="56"/>
-      <c r="AM9" s="54" t="s">
+      <c r="AI9" s="68"/>
+      <c r="AJ9" s="68"/>
+      <c r="AK9" s="68"/>
+      <c r="AL9" s="69"/>
+      <c r="AM9" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="56"/>
-      <c r="AR9" s="54" t="s">
+      <c r="AN9" s="68"/>
+      <c r="AO9" s="68"/>
+      <c r="AP9" s="68"/>
+      <c r="AQ9" s="69"/>
+      <c r="AR9" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
-      <c r="AU9" s="55"/>
-      <c r="AV9" s="56"/>
-      <c r="AW9" s="54" t="s">
+      <c r="AS9" s="68"/>
+      <c r="AT9" s="68"/>
+      <c r="AU9" s="68"/>
+      <c r="AV9" s="69"/>
+      <c r="AW9" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="55"/>
-      <c r="AY9" s="55"/>
-      <c r="AZ9" s="55"/>
-      <c r="BA9" s="56"/>
-      <c r="BB9" s="54" t="s">
+      <c r="AX9" s="68"/>
+      <c r="AY9" s="68"/>
+      <c r="AZ9" s="68"/>
+      <c r="BA9" s="69"/>
+      <c r="BB9" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="55"/>
-      <c r="BD9" s="55"/>
-      <c r="BE9" s="55"/>
-      <c r="BF9" s="56"/>
-      <c r="BG9" s="54" t="s">
+      <c r="BC9" s="68"/>
+      <c r="BD9" s="68"/>
+      <c r="BE9" s="68"/>
+      <c r="BF9" s="69"/>
+      <c r="BG9" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="55"/>
-      <c r="BI9" s="55"/>
-      <c r="BJ9" s="55"/>
-      <c r="BK9" s="56"/>
-      <c r="BL9" s="54" t="s">
+      <c r="BH9" s="68"/>
+      <c r="BI9" s="68"/>
+      <c r="BJ9" s="68"/>
+      <c r="BK9" s="69"/>
+      <c r="BL9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="55"/>
-      <c r="BN9" s="55"/>
-      <c r="BO9" s="55"/>
-      <c r="BP9" s="56"/>
-      <c r="BQ9" s="54" t="s">
+      <c r="BM9" s="68"/>
+      <c r="BN9" s="68"/>
+      <c r="BO9" s="68"/>
+      <c r="BP9" s="69"/>
+      <c r="BQ9" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="55"/>
-      <c r="BS9" s="55"/>
-      <c r="BT9" s="55"/>
-      <c r="BU9" s="56"/>
-      <c r="BV9" s="54" t="s">
+      <c r="BR9" s="68"/>
+      <c r="BS9" s="68"/>
+      <c r="BT9" s="68"/>
+      <c r="BU9" s="69"/>
+      <c r="BV9" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="55"/>
-      <c r="BX9" s="55"/>
-      <c r="BY9" s="55"/>
-      <c r="BZ9" s="56"/>
+      <c r="BW9" s="68"/>
+      <c r="BX9" s="68"/>
+      <c r="BY9" s="68"/>
+      <c r="BZ9" s="69"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="26">
         <v>1</v>
@@ -2037,7 +2043,7 @@
       <c r="BY10" s="29"/>
       <c r="BZ10" s="29"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="33">
         <v>1.1000000000000001</v>
@@ -2132,7 +2138,7 @@
       <c r="BY11" s="38"/>
       <c r="BZ11" s="38"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
       <c r="B12" s="33" t="s">
         <v>13</v>
@@ -2227,7 +2233,7 @@
       <c r="BY12" s="38"/>
       <c r="BZ12" s="38"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="33">
         <v>1.2</v>
@@ -2322,7 +2328,7 @@
       <c r="BY13" s="38"/>
       <c r="BZ13" s="38"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
       <c r="B14" s="33">
         <v>1.3</v>
@@ -2417,7 +2423,7 @@
       <c r="BY14" s="38"/>
       <c r="BZ14" s="38"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
       <c r="B15" s="26">
         <v>2</v>
@@ -2501,7 +2507,7 @@
       <c r="BY15" s="29"/>
       <c r="BZ15" s="29"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
       <c r="B16" s="33">
         <v>2.1</v>
@@ -2603,7 +2609,7 @@
       <c r="BY16" s="38"/>
       <c r="BZ16" s="38"/>
     </row>
-    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32"/>
       <c r="B17" s="33">
         <v>2.2000000000000002</v>
@@ -2692,7 +2698,7 @@
       <c r="BY17" s="38"/>
       <c r="BZ17" s="38"/>
     </row>
-    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="33">
         <v>2.2999999999999998</v>
@@ -2801,7 +2807,7 @@
       <c r="BY18" s="38"/>
       <c r="BZ18" s="38"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32"/>
       <c r="B19" s="33" t="s">
         <v>15</v>
@@ -2907,7 +2913,7 @@
       <c r="BY19" s="38"/>
       <c r="BZ19" s="38"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
       <c r="B20" s="33">
         <v>2.4</v>
@@ -2996,7 +3002,7 @@
       <c r="BY20" s="38"/>
       <c r="BZ20" s="38"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32"/>
       <c r="B21" s="33">
         <v>2.5</v>
@@ -3099,7 +3105,7 @@
       <c r="BY21" s="38"/>
       <c r="BZ21" s="38"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
       <c r="B22" s="33">
         <v>2.6</v>
@@ -3187,7 +3193,7 @@
       <c r="BY22" s="38"/>
       <c r="BZ22" s="38"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32"/>
       <c r="B23" s="33">
         <v>2.7</v>
@@ -3274,7 +3280,7 @@
       <c r="BY23" s="38"/>
       <c r="BZ23" s="38"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32"/>
       <c r="B24" s="33">
         <v>2.8</v>
@@ -3359,7 +3365,7 @@
       <c r="BY24" s="38"/>
       <c r="BZ24" s="38"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32"/>
       <c r="B25" s="33">
         <v>2.9</v>
@@ -3443,7 +3449,7 @@
       <c r="BY25" s="38"/>
       <c r="BZ25" s="38"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32"/>
       <c r="B26" s="46">
         <v>2.1</v>
@@ -3528,7 +3534,7 @@
       <c r="BY26" s="38"/>
       <c r="BZ26" s="38"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32"/>
       <c r="B27" s="46">
         <v>2.11</v>
@@ -3612,7 +3618,7 @@
       <c r="BY27" s="38"/>
       <c r="BZ27" s="38"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32"/>
       <c r="B28" s="26">
         <v>3</v>
@@ -3696,7 +3702,7 @@
       <c r="BY28" s="29"/>
       <c r="BZ28" s="29"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32"/>
       <c r="B29" s="33">
         <v>3.1</v>
@@ -3785,7 +3791,7 @@
       <c r="BY29" s="38"/>
       <c r="BZ29" s="38"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="32"/>
       <c r="B30" s="33">
         <v>3.2</v>
@@ -3873,7 +3879,7 @@
       <c r="BY30" s="38"/>
       <c r="BZ30" s="38"/>
     </row>
-    <row r="31" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
       <c r="B31" s="33" t="s">
         <v>17</v>
@@ -3966,7 +3972,7 @@
       <c r="BY31" s="38"/>
       <c r="BZ31" s="38"/>
     </row>
-    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="32"/>
       <c r="B32" s="33" t="s">
         <v>18</v>
@@ -3982,6 +3988,9 @@
       <c r="G32" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
       </c>
       <c r="I32" s="42"/>
       <c r="J32" s="43"/>
@@ -4054,7 +4063,7 @@
       <c r="BY32" s="38"/>
       <c r="BZ32" s="38"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="32"/>
       <c r="B33" s="33">
         <v>3.3</v>
@@ -4143,7 +4152,7 @@
       <c r="BY33" s="38"/>
       <c r="BZ33" s="38"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32"/>
       <c r="B34" s="33" t="s">
         <v>19</v>
@@ -4233,7 +4242,7 @@
       <c r="BY34" s="38"/>
       <c r="BZ34" s="38"/>
     </row>
-    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
       <c r="B35" s="33"/>
       <c r="C35" s="47" t="s">
@@ -4327,7 +4336,7 @@
       <c r="BY35" s="38"/>
       <c r="BZ35" s="38"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32"/>
       <c r="B36" s="33"/>
       <c r="C36" s="47" t="s">
@@ -4417,7 +4426,7 @@
       <c r="BY36" s="38"/>
       <c r="BZ36" s="38"/>
     </row>
-    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32"/>
       <c r="B37" s="33"/>
       <c r="C37" s="47" t="s">
@@ -4513,7 +4522,7 @@
       <c r="BY37" s="38"/>
       <c r="BZ37" s="38"/>
     </row>
-    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="33"/>
       <c r="C38" s="47" t="s">
         <v>74</v>
@@ -4600,7 +4609,7 @@
       <c r="BY38" s="38"/>
       <c r="BZ38" s="38"/>
     </row>
-    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="33"/>
       <c r="C39" s="47" t="s">
         <v>76</v>
@@ -4687,16 +4696,22 @@
       <c r="BY39" s="38"/>
       <c r="BZ39" s="38"/>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="33"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="34"/>
+      <c r="C40" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>61</v>
+      </c>
       <c r="E40" s="35"/>
       <c r="F40" s="35"/>
       <c r="G40" s="36">
         <v>0</v>
       </c>
-      <c r="H40" s="37"/>
+      <c r="H40" s="37">
+        <v>1</v>
+      </c>
       <c r="I40" s="42"/>
       <c r="J40" s="43"/>
       <c r="K40" s="38"/>
@@ -4768,16 +4783,22 @@
       <c r="BY40" s="38"/>
       <c r="BZ40" s="38"/>
     </row>
-    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="33"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="34"/>
+      <c r="C41" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>61</v>
+      </c>
       <c r="E41" s="35"/>
       <c r="F41" s="35"/>
       <c r="G41" s="36">
         <v>0</v>
       </c>
-      <c r="H41" s="37"/>
+      <c r="H41" s="37">
+        <v>1</v>
+      </c>
       <c r="I41" s="42"/>
       <c r="J41" s="43"/>
       <c r="K41" s="38"/>
@@ -4849,7 +4870,7 @@
       <c r="BY41" s="38"/>
       <c r="BZ41" s="38"/>
     </row>
-    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="26">
         <v>4</v>
       </c>
@@ -4932,7 +4953,7 @@
       <c r="BY42" s="29"/>
       <c r="BZ42" s="29"/>
     </row>
-    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="33">
         <v>4.0999999999999996</v>
       </c>
@@ -5030,7 +5051,7 @@
       <c r="BY43" s="38"/>
       <c r="BZ43" s="38"/>
     </row>
-    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="33">
         <v>4.2</v>
       </c>
@@ -5113,7 +5134,7 @@
       <c r="BY44" s="38"/>
       <c r="BZ44" s="38"/>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="33" t="s">
         <v>42</v>
       </c>
@@ -5197,7 +5218,7 @@
       <c r="BY45" s="38"/>
       <c r="BZ45" s="38"/>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="33" t="s">
         <v>43</v>
       </c>
@@ -5280,7 +5301,7 @@
       <c r="BY46" s="38"/>
       <c r="BZ46" s="38"/>
     </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="33">
         <v>4.3</v>
       </c>
@@ -5364,7 +5385,7 @@
       <c r="BY47" s="38"/>
       <c r="BZ47" s="38"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="33" t="s">
         <v>44</v>
       </c>
@@ -5449,26 +5470,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5485,6 +5486,26 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H48">
     <cfRule type="colorScale" priority="6">
@@ -5512,12 +5533,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5750,15 +5768,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5783,18 +5813,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tested blueprints in final map, updated florcharts and Gantt
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\MoonGame\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744B036D-CFCC-4AD1-BAE8-40064D1A4954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E0A4B2-6FB9-4155-AF03-BFC8103EB274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="81">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -790,54 +790,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -855,6 +807,54 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1176,22 +1176,22 @@
   </sheetPr>
   <dimension ref="A1:BZ50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BQ38" sqref="BQ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" customWidth="1"/>
-    <col min="9" max="78" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="9" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1271,40 +1271,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1353,7 +1353,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1433,43 +1433,43 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="65" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="66" t="s">
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="63"/>
+      <c r="Z4" s="63"/>
+      <c r="AA4" s="63"/>
+      <c r="AB4" s="63"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -1521,42 +1521,42 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="58">
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="75">
         <v>44802</v>
       </c>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="57"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="63"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -1609,7 +1609,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
         <v>48</v>
@@ -1691,7 +1691,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1771,209 +1771,209 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="67" t="s">
+      <c r="H8" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="49"/>
-      <c r="Z8" s="49"/>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="49"/>
-      <c r="AC8" s="49"/>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="49"/>
-      <c r="AF8" s="49"/>
-      <c r="AG8" s="49"/>
-      <c r="AH8" s="49"/>
-      <c r="AI8" s="49"/>
-      <c r="AJ8" s="49"/>
-      <c r="AK8" s="49"/>
-      <c r="AL8" s="49"/>
-      <c r="AM8" s="48"/>
-      <c r="AN8" s="49"/>
-      <c r="AO8" s="49"/>
-      <c r="AP8" s="49"/>
-      <c r="AQ8" s="49"/>
-      <c r="AR8" s="49"/>
-      <c r="AS8" s="49"/>
-      <c r="AT8" s="49"/>
-      <c r="AU8" s="49"/>
-      <c r="AV8" s="49"/>
-      <c r="AW8" s="49"/>
-      <c r="AX8" s="49"/>
-      <c r="AY8" s="49"/>
-      <c r="AZ8" s="49"/>
-      <c r="BA8" s="49"/>
-      <c r="BB8" s="48"/>
-      <c r="BC8" s="49"/>
-      <c r="BD8" s="49"/>
-      <c r="BE8" s="49"/>
-      <c r="BF8" s="49"/>
-      <c r="BG8" s="49"/>
-      <c r="BH8" s="49"/>
-      <c r="BI8" s="49"/>
-      <c r="BJ8" s="49"/>
-      <c r="BK8" s="49"/>
-      <c r="BL8" s="49"/>
-      <c r="BM8" s="49"/>
-      <c r="BN8" s="49"/>
-      <c r="BO8" s="49"/>
-      <c r="BP8" s="49"/>
-      <c r="BQ8" s="49"/>
-      <c r="BR8" s="49"/>
-      <c r="BS8" s="49"/>
-      <c r="BT8" s="49"/>
-      <c r="BU8" s="49"/>
-      <c r="BV8" s="49"/>
-      <c r="BW8" s="49"/>
-      <c r="BX8" s="49"/>
-      <c r="BY8" s="49"/>
-      <c r="BZ8" s="50"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
+      <c r="V8" s="68"/>
+      <c r="W8" s="68"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="68"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="68"/>
+      <c r="AD8" s="68"/>
+      <c r="AE8" s="68"/>
+      <c r="AF8" s="68"/>
+      <c r="AG8" s="68"/>
+      <c r="AH8" s="68"/>
+      <c r="AI8" s="68"/>
+      <c r="AJ8" s="68"/>
+      <c r="AK8" s="68"/>
+      <c r="AL8" s="68"/>
+      <c r="AM8" s="69"/>
+      <c r="AN8" s="68"/>
+      <c r="AO8" s="68"/>
+      <c r="AP8" s="68"/>
+      <c r="AQ8" s="68"/>
+      <c r="AR8" s="68"/>
+      <c r="AS8" s="68"/>
+      <c r="AT8" s="68"/>
+      <c r="AU8" s="68"/>
+      <c r="AV8" s="68"/>
+      <c r="AW8" s="68"/>
+      <c r="AX8" s="68"/>
+      <c r="AY8" s="68"/>
+      <c r="AZ8" s="68"/>
+      <c r="BA8" s="68"/>
+      <c r="BB8" s="69"/>
+      <c r="BC8" s="68"/>
+      <c r="BD8" s="68"/>
+      <c r="BE8" s="68"/>
+      <c r="BF8" s="68"/>
+      <c r="BG8" s="68"/>
+      <c r="BH8" s="68"/>
+      <c r="BI8" s="68"/>
+      <c r="BJ8" s="68"/>
+      <c r="BK8" s="68"/>
+      <c r="BL8" s="68"/>
+      <c r="BM8" s="68"/>
+      <c r="BN8" s="68"/>
+      <c r="BO8" s="68"/>
+      <c r="BP8" s="68"/>
+      <c r="BQ8" s="68"/>
+      <c r="BR8" s="68"/>
+      <c r="BS8" s="68"/>
+      <c r="BT8" s="68"/>
+      <c r="BU8" s="68"/>
+      <c r="BV8" s="68"/>
+      <c r="BW8" s="68"/>
+      <c r="BX8" s="68"/>
+      <c r="BY8" s="68"/>
+      <c r="BZ8" s="73"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="51" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="51" t="s">
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="51" t="s">
+      <c r="O9" s="71"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="53"/>
-      <c r="X9" s="51" t="s">
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="72"/>
+      <c r="X9" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="53"/>
-      <c r="AC9" s="51" t="s">
+      <c r="Y9" s="71"/>
+      <c r="Z9" s="71"/>
+      <c r="AA9" s="71"/>
+      <c r="AB9" s="72"/>
+      <c r="AC9" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="52"/>
-      <c r="AE9" s="52"/>
-      <c r="AF9" s="52"/>
-      <c r="AG9" s="53"/>
-      <c r="AH9" s="51" t="s">
+      <c r="AD9" s="71"/>
+      <c r="AE9" s="71"/>
+      <c r="AF9" s="71"/>
+      <c r="AG9" s="72"/>
+      <c r="AH9" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="52"/>
-      <c r="AJ9" s="52"/>
-      <c r="AK9" s="52"/>
-      <c r="AL9" s="53"/>
-      <c r="AM9" s="51" t="s">
+      <c r="AI9" s="71"/>
+      <c r="AJ9" s="71"/>
+      <c r="AK9" s="71"/>
+      <c r="AL9" s="72"/>
+      <c r="AM9" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="52"/>
-      <c r="AO9" s="52"/>
-      <c r="AP9" s="52"/>
-      <c r="AQ9" s="53"/>
-      <c r="AR9" s="51" t="s">
+      <c r="AN9" s="71"/>
+      <c r="AO9" s="71"/>
+      <c r="AP9" s="71"/>
+      <c r="AQ9" s="72"/>
+      <c r="AR9" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="52"/>
-      <c r="AT9" s="52"/>
-      <c r="AU9" s="52"/>
-      <c r="AV9" s="53"/>
-      <c r="AW9" s="51" t="s">
+      <c r="AS9" s="71"/>
+      <c r="AT9" s="71"/>
+      <c r="AU9" s="71"/>
+      <c r="AV9" s="72"/>
+      <c r="AW9" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="52"/>
-      <c r="AY9" s="52"/>
-      <c r="AZ9" s="52"/>
-      <c r="BA9" s="53"/>
-      <c r="BB9" s="51" t="s">
+      <c r="AX9" s="71"/>
+      <c r="AY9" s="71"/>
+      <c r="AZ9" s="71"/>
+      <c r="BA9" s="72"/>
+      <c r="BB9" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="52"/>
-      <c r="BD9" s="52"/>
-      <c r="BE9" s="52"/>
-      <c r="BF9" s="53"/>
-      <c r="BG9" s="51" t="s">
+      <c r="BC9" s="71"/>
+      <c r="BD9" s="71"/>
+      <c r="BE9" s="71"/>
+      <c r="BF9" s="72"/>
+      <c r="BG9" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="52"/>
-      <c r="BI9" s="52"/>
-      <c r="BJ9" s="52"/>
-      <c r="BK9" s="53"/>
-      <c r="BL9" s="51" t="s">
+      <c r="BH9" s="71"/>
+      <c r="BI9" s="71"/>
+      <c r="BJ9" s="71"/>
+      <c r="BK9" s="72"/>
+      <c r="BL9" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="52"/>
-      <c r="BN9" s="52"/>
-      <c r="BO9" s="52"/>
-      <c r="BP9" s="53"/>
-      <c r="BQ9" s="51" t="s">
+      <c r="BM9" s="71"/>
+      <c r="BN9" s="71"/>
+      <c r="BO9" s="71"/>
+      <c r="BP9" s="72"/>
+      <c r="BQ9" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="52"/>
-      <c r="BS9" s="52"/>
-      <c r="BT9" s="52"/>
-      <c r="BU9" s="53"/>
-      <c r="BV9" s="51" t="s">
+      <c r="BR9" s="71"/>
+      <c r="BS9" s="71"/>
+      <c r="BT9" s="71"/>
+      <c r="BU9" s="72"/>
+      <c r="BV9" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="52"/>
-      <c r="BX9" s="52"/>
-      <c r="BY9" s="52"/>
-      <c r="BZ9" s="53"/>
+      <c r="BW9" s="71"/>
+      <c r="BX9" s="71"/>
+      <c r="BY9" s="71"/>
+      <c r="BZ9" s="72"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="26">
         <v>1</v>
@@ -2057,7 +2057,7 @@
       <c r="BY10" s="29"/>
       <c r="BZ10" s="29"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="33">
         <v>1.1000000000000001</v>
@@ -2152,7 +2152,7 @@
       <c r="BY11" s="38"/>
       <c r="BZ11" s="38"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
       <c r="B12" s="33" t="s">
         <v>13</v>
@@ -2247,7 +2247,7 @@
       <c r="BY12" s="38"/>
       <c r="BZ12" s="38"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="33">
         <v>1.2</v>
@@ -2342,7 +2342,7 @@
       <c r="BY13" s="38"/>
       <c r="BZ13" s="38"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
       <c r="B14" s="33">
         <v>1.3</v>
@@ -2437,7 +2437,7 @@
       <c r="BY14" s="38"/>
       <c r="BZ14" s="38"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
       <c r="B15" s="26">
         <v>2</v>
@@ -2521,12 +2521,12 @@
       <c r="BY15" s="29"/>
       <c r="BZ15" s="29"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
       <c r="B16" s="33">
         <v>2.1</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="48" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="34" t="s">
@@ -2539,7 +2539,7 @@
       <c r="G16" s="36">
         <v>0</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="49">
         <v>0.75</v>
       </c>
       <c r="I16" s="42"/>
@@ -2623,12 +2623,12 @@
       <c r="BY16" s="38"/>
       <c r="BZ16" s="38"/>
     </row>
-    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32"/>
       <c r="B17" s="33">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="50" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="34" t="s">
@@ -2640,7 +2640,7 @@
         <f t="shared" ref="G17:G18" si="1">DAYS360(E17,F17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="72"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="42"/>
       <c r="J17" s="43"/>
       <c r="K17" s="38"/>
@@ -2712,12 +2712,12 @@
       <c r="BY17" s="38"/>
       <c r="BZ17" s="38"/>
     </row>
-    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="50" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="34" t="s">
@@ -2731,7 +2731,7 @@
         <f t="shared" si="1"/>
         <v>-44186</v>
       </c>
-      <c r="H18" s="73">
+      <c r="H18" s="51">
         <v>0.5</v>
       </c>
       <c r="I18" s="42"/>
@@ -2821,12 +2821,12 @@
       <c r="BY18" s="38"/>
       <c r="BZ18" s="38"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32"/>
       <c r="B19" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="50" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="34" t="s">
@@ -2839,7 +2839,7 @@
       <c r="G19" s="36">
         <v>0</v>
       </c>
-      <c r="H19" s="73">
+      <c r="H19" s="51">
         <v>0.25</v>
       </c>
       <c r="I19" s="42"/>
@@ -2927,12 +2927,12 @@
       <c r="BY19" s="38"/>
       <c r="BZ19" s="38"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
       <c r="B20" s="33">
         <v>2.4</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="50" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="34" t="s">
@@ -2944,7 +2944,7 @@
         <f t="shared" ref="G20:G21" si="2">DAYS360(E20,F20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="72"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="42"/>
       <c r="J20" s="43"/>
       <c r="K20" s="38"/>
@@ -3016,12 +3016,12 @@
       <c r="BY20" s="38"/>
       <c r="BZ20" s="38"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32"/>
       <c r="B21" s="33">
         <v>2.5</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="50" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="34" t="s">
@@ -3035,7 +3035,7 @@
         <f t="shared" si="2"/>
         <v>-44179</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="51">
         <v>0.25</v>
       </c>
       <c r="I21" s="42"/>
@@ -3119,12 +3119,12 @@
       <c r="BY21" s="38"/>
       <c r="BZ21" s="38"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
       <c r="B22" s="33">
         <v>2.6</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="50" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="34" t="s">
@@ -3135,7 +3135,7 @@
       <c r="G22" s="36">
         <v>0</v>
       </c>
-      <c r="H22" s="72"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="42"/>
       <c r="J22" s="43"/>
       <c r="K22" s="38"/>
@@ -3207,12 +3207,12 @@
       <c r="BY22" s="38"/>
       <c r="BZ22" s="38"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32"/>
       <c r="B23" s="33">
         <v>2.7</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="50" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="34"/>
@@ -3222,7 +3222,7 @@
         <f t="shared" ref="G23:G24" si="3">DAYS360(E23,F23)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="72"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="42"/>
       <c r="J23" s="43"/>
       <c r="K23" s="38"/>
@@ -3294,12 +3294,12 @@
       <c r="BY23" s="38"/>
       <c r="BZ23" s="38"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32"/>
       <c r="B24" s="33">
         <v>2.8</v>
       </c>
-      <c r="C24" s="72"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="34"/>
       <c r="E24" s="35"/>
       <c r="F24" s="35"/>
@@ -3307,7 +3307,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H24" s="72"/>
+      <c r="H24" s="50"/>
       <c r="I24" s="42"/>
       <c r="J24" s="43"/>
       <c r="K24" s="38"/>
@@ -3379,19 +3379,19 @@
       <c r="BY24" s="38"/>
       <c r="BZ24" s="38"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32"/>
       <c r="B25" s="33">
         <v>2.9</v>
       </c>
-      <c r="C25" s="72"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="34"/>
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
       <c r="G25" s="36">
         <v>0</v>
       </c>
-      <c r="H25" s="72"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="42"/>
       <c r="J25" s="43"/>
       <c r="K25" s="38"/>
@@ -3463,12 +3463,12 @@
       <c r="BY25" s="38"/>
       <c r="BZ25" s="38"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32"/>
       <c r="B26" s="46">
         <v>2.1</v>
       </c>
-      <c r="C26" s="72"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
@@ -3476,7 +3476,7 @@
         <f>DAYS360(E26,F26)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="72"/>
+      <c r="H26" s="50"/>
       <c r="I26" s="42"/>
       <c r="J26" s="43"/>
       <c r="K26" s="38"/>
@@ -3548,19 +3548,19 @@
       <c r="BY26" s="38"/>
       <c r="BZ26" s="38"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32"/>
       <c r="B27" s="46">
         <v>2.11</v>
       </c>
-      <c r="C27" s="72"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="34"/>
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
       <c r="G27" s="36">
         <v>0</v>
       </c>
-      <c r="H27" s="72"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="42"/>
       <c r="J27" s="43"/>
       <c r="K27" s="38"/>
@@ -3632,7 +3632,7 @@
       <c r="BY27" s="38"/>
       <c r="BZ27" s="38"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32"/>
       <c r="B28" s="26">
         <v>3</v>
@@ -3716,12 +3716,12 @@
       <c r="BY28" s="29"/>
       <c r="BZ28" s="29"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32"/>
       <c r="B29" s="33">
         <v>3.1</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="50" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="34" t="s">
@@ -3805,12 +3805,12 @@
       <c r="BY29" s="38"/>
       <c r="BZ29" s="38"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="32"/>
       <c r="B30" s="33">
         <v>3.2</v>
       </c>
-      <c r="C30" s="72" t="s">
+      <c r="C30" s="50" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="34" t="s">
@@ -3893,10 +3893,10 @@
       <c r="BY30" s="38"/>
       <c r="BZ30" s="38"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32"/>
       <c r="B31" s="33"/>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="48" t="s">
         <v>80</v>
       </c>
       <c r="D31" s="34" t="s">
@@ -3909,7 +3909,7 @@
       <c r="G31" s="36">
         <v>0</v>
       </c>
-      <c r="H31" s="74">
+      <c r="H31" s="52">
         <v>100</v>
       </c>
       <c r="I31" s="42"/>
@@ -3991,12 +3991,12 @@
       <c r="BY31" s="38"/>
       <c r="BZ31" s="38"/>
     </row>
-    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
       <c r="B32" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="50" t="s">
         <v>58</v>
       </c>
       <c r="D32" s="34" t="s">
@@ -4010,7 +4010,7 @@
         <f t="shared" ref="G32:G34" si="4">DAYS360(E32,F32)</f>
         <v>-44206</v>
       </c>
-      <c r="H32" s="74">
+      <c r="H32" s="52">
         <v>90</v>
       </c>
       <c r="I32" s="42"/>
@@ -4104,12 +4104,12 @@
       <c r="BY32" s="38"/>
       <c r="BZ32" s="38"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="32"/>
       <c r="B33" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="50" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="34" t="s">
@@ -4121,7 +4121,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H33" s="74">
+      <c r="H33" s="52">
         <v>100</v>
       </c>
       <c r="I33" s="42"/>
@@ -4195,12 +4195,12 @@
       <c r="BY33" s="38"/>
       <c r="BZ33" s="38"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32"/>
       <c r="B34" s="33">
         <v>3.3</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="50" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="34" t="s">
@@ -4212,7 +4212,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H34" s="74"/>
+      <c r="H34" s="52"/>
       <c r="I34" s="42"/>
       <c r="J34" s="43"/>
       <c r="K34" s="38"/>
@@ -4284,12 +4284,12 @@
       <c r="BY34" s="38"/>
       <c r="BZ34" s="38"/>
     </row>
-    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32"/>
       <c r="B35" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="72" t="s">
+      <c r="C35" s="50" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="34" t="s">
@@ -4301,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="37">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I35" s="42"/>
       <c r="J35" s="43"/>
@@ -4325,33 +4325,59 @@
       <c r="AB35" s="38"/>
       <c r="AC35" s="39"/>
       <c r="AD35" s="39"/>
-      <c r="AE35" s="39"/>
+      <c r="AE35" s="39" t="s">
+        <v>71</v>
+      </c>
       <c r="AF35" s="39"/>
-      <c r="AG35" s="39"/>
-      <c r="AH35" s="38"/>
+      <c r="AG35" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="AI35" s="38"/>
-      <c r="AJ35" s="38"/>
-      <c r="AK35" s="38"/>
-      <c r="AL35" s="38"/>
+      <c r="AJ35" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK35" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="AM35" s="38"/>
       <c r="AN35" s="38"/>
       <c r="AO35" s="38"/>
-      <c r="AP35" s="38"/>
+      <c r="AP35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="AQ35" s="38"/>
       <c r="AR35" s="40"/>
       <c r="AS35" s="40"/>
-      <c r="AT35" s="40"/>
-      <c r="AU35" s="40"/>
-      <c r="AV35" s="40"/>
+      <c r="AT35" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU35" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV35" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="AW35" s="38"/>
       <c r="AX35" s="38"/>
-      <c r="AY35" s="38"/>
+      <c r="AY35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ35" s="38"/>
       <c r="BA35" s="38"/>
-      <c r="BB35" s="38"/>
+      <c r="BB35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="BC35" s="38"/>
       <c r="BD35" s="38"/>
-      <c r="BE35" s="38"/>
+      <c r="BE35" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="BF35" s="38"/>
       <c r="BG35" s="41"/>
       <c r="BH35" s="41"/>
@@ -4374,10 +4400,10 @@
       <c r="BY35" s="38"/>
       <c r="BZ35" s="38"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32"/>
       <c r="B36" s="33"/>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="50" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="34" t="s">
@@ -4476,10 +4502,10 @@
       <c r="BY36" s="38"/>
       <c r="BZ36" s="38"/>
     </row>
-    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32"/>
       <c r="B37" s="33"/>
-      <c r="C37" s="72" t="s">
+      <c r="C37" s="50" t="s">
         <v>68</v>
       </c>
       <c r="D37" s="34" t="s">
@@ -4566,10 +4592,10 @@
       <c r="BY37" s="38"/>
       <c r="BZ37" s="38"/>
     </row>
-    <row r="38" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="33"/>
-      <c r="C38" s="72" t="s">
+      <c r="C38" s="50" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="34" t="s">
@@ -4583,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="37">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="I38" s="42"/>
       <c r="J38" s="43"/>
@@ -4633,24 +4659,42 @@
       <c r="AV38" s="40"/>
       <c r="AW38" s="38"/>
       <c r="AX38" s="38"/>
-      <c r="AY38" s="38"/>
+      <c r="AY38" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ38" s="38"/>
-      <c r="BA38" s="38"/>
-      <c r="BB38" s="38"/>
+      <c r="BA38" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB38" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="BC38" s="38"/>
       <c r="BD38" s="38"/>
-      <c r="BE38" s="38"/>
-      <c r="BF38" s="38"/>
-      <c r="BG38" s="41"/>
+      <c r="BE38" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF38" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG38" s="41" t="s">
+        <v>71</v>
+      </c>
       <c r="BH38" s="41"/>
       <c r="BI38" s="41"/>
       <c r="BJ38" s="41"/>
-      <c r="BK38" s="41"/>
-      <c r="BL38" s="38"/>
+      <c r="BK38" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL38" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="BM38" s="38"/>
       <c r="BN38" s="38"/>
       <c r="BO38" s="38"/>
-      <c r="BP38" s="38"/>
+      <c r="BP38" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="BQ38" s="38"/>
       <c r="BR38" s="38"/>
       <c r="BS38" s="38"/>
@@ -4662,22 +4706,22 @@
       <c r="BY38" s="38"/>
       <c r="BZ38" s="38"/>
     </row>
-    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="33"/>
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="50" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="75">
+      <c r="E39" s="53">
         <v>44872</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="36">
         <v>0</v>
       </c>
-      <c r="H39" s="74">
+      <c r="H39" s="52">
         <v>80</v>
       </c>
       <c r="I39" s="42"/>
@@ -4753,22 +4797,22 @@
       <c r="BY39" s="38"/>
       <c r="BZ39" s="38"/>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="33"/>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="50" t="s">
         <v>75</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="75">
+      <c r="E40" s="53">
         <v>44873</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="36">
         <v>0</v>
       </c>
-      <c r="H40" s="74">
+      <c r="H40" s="52">
         <v>20</v>
       </c>
       <c r="I40" s="42"/>
@@ -4850,9 +4894,9 @@
       <c r="BY40" s="38"/>
       <c r="BZ40" s="38"/>
     </row>
-    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="33"/>
-      <c r="C41" s="72" t="s">
+      <c r="C41" s="50" t="s">
         <v>77</v>
       </c>
       <c r="D41" s="34" t="s">
@@ -4937,9 +4981,9 @@
       <c r="BY41" s="38"/>
       <c r="BZ41" s="38"/>
     </row>
-    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="33"/>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="50" t="s">
         <v>78</v>
       </c>
       <c r="D42" s="34" t="s">
@@ -5024,9 +5068,9 @@
       <c r="BY42" s="38"/>
       <c r="BZ42" s="38"/>
     </row>
-    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="33"/>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="48" t="s">
         <v>79</v>
       </c>
       <c r="D43" s="34" t="s">
@@ -5037,7 +5081,7 @@
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="36"/>
-      <c r="H43" s="74">
+      <c r="H43" s="52">
         <v>100</v>
       </c>
       <c r="I43" s="42"/>
@@ -5121,7 +5165,7 @@
       <c r="BY43" s="38"/>
       <c r="BZ43" s="38"/>
     </row>
-    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="26">
         <v>4</v>
       </c>
@@ -5204,11 +5248,11 @@
       <c r="BY44" s="29"/>
       <c r="BZ44" s="29"/>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="33">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C45" s="72" t="s">
+      <c r="C45" s="50" t="s">
         <v>72</v>
       </c>
       <c r="D45" s="34" t="s">
@@ -5302,11 +5346,11 @@
       <c r="BY45" s="38"/>
       <c r="BZ45" s="38"/>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="33">
         <v>4.2</v>
       </c>
-      <c r="C46" s="72"/>
+      <c r="C46" s="50"/>
       <c r="D46" s="34"/>
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
@@ -5385,11 +5429,11 @@
       <c r="BY46" s="38"/>
       <c r="BZ46" s="38"/>
     </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="72"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="34"/>
       <c r="E47" s="35"/>
       <c r="F47" s="35"/>
@@ -5469,11 +5513,11 @@
       <c r="BY47" s="38"/>
       <c r="BZ47" s="38"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="72"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="34"/>
       <c r="E48" s="35"/>
       <c r="F48" s="35"/>
@@ -5481,7 +5525,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H48" s="74"/>
+      <c r="H48" s="52"/>
       <c r="I48" s="42"/>
       <c r="J48" s="43"/>
       <c r="K48" s="38"/>
@@ -5553,11 +5597,11 @@
       <c r="BY48" s="38"/>
       <c r="BZ48" s="38"/>
     </row>
-    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="33">
         <v>4.3</v>
       </c>
-      <c r="C49" s="72"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="34"/>
       <c r="E49" s="35"/>
       <c r="F49" s="35"/>
@@ -5637,7 +5681,7 @@
       <c r="BY49" s="38"/>
       <c r="BZ49" s="38"/>
     </row>
-    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="33" t="s">
         <v>44</v>
       </c>
@@ -5722,26 +5766,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5758,6 +5782,26 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H50">
     <cfRule type="colorScale" priority="6">
@@ -5785,12 +5829,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6023,15 +6064,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6056,18 +6109,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement Puzzles in Final Map
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8EDE40-5B91-4DEC-A6B1-5822807EE6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33463DE-EB33-4634-8E04-756456C5BB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -768,66 +768,6 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -848,6 +788,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,8 +1169,8 @@
   </sheetPr>
   <dimension ref="A1:BZ50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1266,38 +1266,38 @@
     </row>
     <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1428,41 +1428,41 @@
     </row>
     <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="52" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="53" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="56"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -1516,40 +1516,40 @@
     </row>
     <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="46">
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="68">
         <v>44802</v>
       </c>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="56"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -1784,201 +1784,201 @@
       <c r="G8" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="40"/>
-      <c r="Y8" s="56"/>
-      <c r="Z8" s="56"/>
-      <c r="AA8" s="56"/>
-      <c r="AB8" s="56"/>
-      <c r="AC8" s="56"/>
-      <c r="AD8" s="56"/>
-      <c r="AE8" s="56"/>
-      <c r="AF8" s="56"/>
-      <c r="AG8" s="56"/>
-      <c r="AH8" s="56"/>
-      <c r="AI8" s="56"/>
-      <c r="AJ8" s="56"/>
-      <c r="AK8" s="56"/>
-      <c r="AL8" s="56"/>
-      <c r="AM8" s="40"/>
-      <c r="AN8" s="56"/>
-      <c r="AO8" s="56"/>
-      <c r="AP8" s="56"/>
-      <c r="AQ8" s="56"/>
-      <c r="AR8" s="56"/>
-      <c r="AS8" s="56"/>
-      <c r="AT8" s="56"/>
-      <c r="AU8" s="56"/>
-      <c r="AV8" s="56"/>
-      <c r="AW8" s="56"/>
-      <c r="AX8" s="56"/>
-      <c r="AY8" s="56"/>
-      <c r="AZ8" s="56"/>
-      <c r="BA8" s="56"/>
-      <c r="BB8" s="40"/>
-      <c r="BC8" s="56"/>
-      <c r="BD8" s="56"/>
-      <c r="BE8" s="56"/>
-      <c r="BF8" s="56"/>
-      <c r="BG8" s="56"/>
-      <c r="BH8" s="56"/>
-      <c r="BI8" s="56"/>
-      <c r="BJ8" s="56"/>
-      <c r="BK8" s="56"/>
-      <c r="BL8" s="56"/>
-      <c r="BM8" s="56"/>
-      <c r="BN8" s="56"/>
-      <c r="BO8" s="56"/>
-      <c r="BP8" s="56"/>
-      <c r="BQ8" s="56"/>
-      <c r="BR8" s="56"/>
-      <c r="BS8" s="56"/>
-      <c r="BT8" s="56"/>
-      <c r="BU8" s="56"/>
-      <c r="BV8" s="56"/>
-      <c r="BW8" s="56"/>
-      <c r="BX8" s="56"/>
-      <c r="BY8" s="56"/>
-      <c r="BZ8" s="57"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="61"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="61"/>
+      <c r="AA8" s="61"/>
+      <c r="AB8" s="61"/>
+      <c r="AC8" s="61"/>
+      <c r="AD8" s="61"/>
+      <c r="AE8" s="61"/>
+      <c r="AF8" s="61"/>
+      <c r="AG8" s="61"/>
+      <c r="AH8" s="61"/>
+      <c r="AI8" s="61"/>
+      <c r="AJ8" s="61"/>
+      <c r="AK8" s="61"/>
+      <c r="AL8" s="61"/>
+      <c r="AM8" s="62"/>
+      <c r="AN8" s="61"/>
+      <c r="AO8" s="61"/>
+      <c r="AP8" s="61"/>
+      <c r="AQ8" s="61"/>
+      <c r="AR8" s="61"/>
+      <c r="AS8" s="61"/>
+      <c r="AT8" s="61"/>
+      <c r="AU8" s="61"/>
+      <c r="AV8" s="61"/>
+      <c r="AW8" s="61"/>
+      <c r="AX8" s="61"/>
+      <c r="AY8" s="61"/>
+      <c r="AZ8" s="61"/>
+      <c r="BA8" s="61"/>
+      <c r="BB8" s="62"/>
+      <c r="BC8" s="61"/>
+      <c r="BD8" s="61"/>
+      <c r="BE8" s="61"/>
+      <c r="BF8" s="61"/>
+      <c r="BG8" s="61"/>
+      <c r="BH8" s="61"/>
+      <c r="BI8" s="61"/>
+      <c r="BJ8" s="61"/>
+      <c r="BK8" s="61"/>
+      <c r="BL8" s="61"/>
+      <c r="BM8" s="61"/>
+      <c r="BN8" s="61"/>
+      <c r="BO8" s="61"/>
+      <c r="BP8" s="61"/>
+      <c r="BQ8" s="61"/>
+      <c r="BR8" s="61"/>
+      <c r="BS8" s="61"/>
+      <c r="BT8" s="61"/>
+      <c r="BU8" s="61"/>
+      <c r="BV8" s="61"/>
+      <c r="BW8" s="61"/>
+      <c r="BX8" s="61"/>
+      <c r="BY8" s="61"/>
+      <c r="BZ8" s="66"/>
     </row>
     <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="59"/>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="41" t="s">
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="41" t="s">
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="41" t="s">
+      <c r="T9" s="64"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="65"/>
+      <c r="X9" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="41" t="s">
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="64"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="65"/>
+      <c r="AC9" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="61"/>
-      <c r="AH9" s="41" t="s">
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="64"/>
+      <c r="AF9" s="64"/>
+      <c r="AG9" s="65"/>
+      <c r="AH9" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="60"/>
-      <c r="AJ9" s="60"/>
-      <c r="AK9" s="60"/>
-      <c r="AL9" s="61"/>
-      <c r="AM9" s="41" t="s">
+      <c r="AI9" s="64"/>
+      <c r="AJ9" s="64"/>
+      <c r="AK9" s="64"/>
+      <c r="AL9" s="65"/>
+      <c r="AM9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="60"/>
-      <c r="AO9" s="60"/>
-      <c r="AP9" s="60"/>
-      <c r="AQ9" s="61"/>
-      <c r="AR9" s="41" t="s">
+      <c r="AN9" s="64"/>
+      <c r="AO9" s="64"/>
+      <c r="AP9" s="64"/>
+      <c r="AQ9" s="65"/>
+      <c r="AR9" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="60"/>
-      <c r="AT9" s="60"/>
-      <c r="AU9" s="60"/>
-      <c r="AV9" s="61"/>
-      <c r="AW9" s="41" t="s">
+      <c r="AS9" s="64"/>
+      <c r="AT9" s="64"/>
+      <c r="AU9" s="64"/>
+      <c r="AV9" s="65"/>
+      <c r="AW9" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="60"/>
-      <c r="AY9" s="60"/>
-      <c r="AZ9" s="60"/>
-      <c r="BA9" s="61"/>
-      <c r="BB9" s="41" t="s">
+      <c r="AX9" s="64"/>
+      <c r="AY9" s="64"/>
+      <c r="AZ9" s="64"/>
+      <c r="BA9" s="65"/>
+      <c r="BB9" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="60"/>
-      <c r="BD9" s="60"/>
-      <c r="BE9" s="60"/>
-      <c r="BF9" s="61"/>
-      <c r="BG9" s="41" t="s">
+      <c r="BC9" s="64"/>
+      <c r="BD9" s="64"/>
+      <c r="BE9" s="64"/>
+      <c r="BF9" s="65"/>
+      <c r="BG9" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="60"/>
-      <c r="BI9" s="60"/>
-      <c r="BJ9" s="60"/>
-      <c r="BK9" s="61"/>
-      <c r="BL9" s="41" t="s">
+      <c r="BH9" s="64"/>
+      <c r="BI9" s="64"/>
+      <c r="BJ9" s="64"/>
+      <c r="BK9" s="65"/>
+      <c r="BL9" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="60"/>
-      <c r="BN9" s="60"/>
-      <c r="BO9" s="60"/>
-      <c r="BP9" s="61"/>
-      <c r="BQ9" s="41" t="s">
+      <c r="BM9" s="64"/>
+      <c r="BN9" s="64"/>
+      <c r="BO9" s="64"/>
+      <c r="BP9" s="65"/>
+      <c r="BQ9" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="60"/>
-      <c r="BS9" s="60"/>
-      <c r="BT9" s="60"/>
-      <c r="BU9" s="61"/>
-      <c r="BV9" s="41" t="s">
+      <c r="BR9" s="64"/>
+      <c r="BS9" s="64"/>
+      <c r="BT9" s="64"/>
+      <c r="BU9" s="65"/>
+      <c r="BV9" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="BW9" s="60"/>
-      <c r="BX9" s="60"/>
-      <c r="BY9" s="60"/>
-      <c r="BZ9" s="61"/>
+      <c r="BW9" s="64"/>
+      <c r="BX9" s="64"/>
+      <c r="BY9" s="64"/>
+      <c r="BZ9" s="65"/>
     </row>
     <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="62">
+      <c r="B10" s="40">
         <v>1</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="26"/>
       <c r="J10" s="27"/>
       <c r="K10" s="28"/>
@@ -2061,17 +2061,17 @@
       <c r="D11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="41">
         <v>44809</v>
       </c>
-      <c r="F11" s="63">
+      <c r="F11" s="41">
         <v>44809</v>
       </c>
       <c r="G11" s="30">
         <f t="shared" ref="G11:G14" si="0">DAYS360(E11,F11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="64">
+      <c r="H11" s="42">
         <v>100</v>
       </c>
       <c r="I11" s="32"/>
@@ -2156,17 +2156,17 @@
       <c r="D12" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="41">
         <v>44809</v>
       </c>
-      <c r="F12" s="63">
+      <c r="F12" s="41">
         <v>44809</v>
       </c>
       <c r="G12" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="64">
+      <c r="H12" s="42">
         <v>100</v>
       </c>
       <c r="I12" s="32"/>
@@ -2251,17 +2251,17 @@
       <c r="D13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="41">
         <v>44809</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="41">
         <v>44809</v>
       </c>
       <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="42">
         <v>100</v>
       </c>
       <c r="I13" s="32"/>
@@ -2346,17 +2346,17 @@
       <c r="D14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="41">
         <v>44809</v>
       </c>
-      <c r="F14" s="63">
+      <c r="F14" s="41">
         <v>44809</v>
       </c>
       <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="64">
+      <c r="H14" s="42">
         <v>100</v>
       </c>
       <c r="I14" s="32"/>
@@ -2432,17 +2432,17 @@
     </row>
     <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
-      <c r="B15" s="62">
+      <c r="B15" s="40">
         <v>2</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="26"/>
       <c r="J15" s="27"/>
       <c r="K15" s="28"/>
@@ -2519,20 +2519,20 @@
       <c r="B16" s="30">
         <v>2.1</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="43" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="63">
+      <c r="E16" s="41">
         <v>44851</v>
       </c>
-      <c r="F16" s="63"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="30">
         <v>0</v>
       </c>
-      <c r="H16" s="64">
+      <c r="H16" s="42">
         <v>75</v>
       </c>
       <c r="I16" s="36"/>
@@ -2621,21 +2621,21 @@
       <c r="B17" s="30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="44" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="41">
         <v>44830</v>
       </c>
-      <c r="F17" s="63"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="30">
         <f t="shared" ref="G17" si="1">DAYS360(E17,F17)</f>
         <v>-44186</v>
       </c>
-      <c r="H17" s="64">
+      <c r="H17" s="42">
         <v>50</v>
       </c>
       <c r="I17" s="36"/>
@@ -2730,20 +2730,20 @@
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="44" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="41">
         <v>44840</v>
       </c>
-      <c r="F18" s="63"/>
+      <c r="F18" s="41"/>
       <c r="G18" s="30">
         <v>0</v>
       </c>
-      <c r="H18" s="64">
+      <c r="H18" s="42">
         <v>25</v>
       </c>
       <c r="I18" s="36"/>
@@ -2836,21 +2836,21 @@
       <c r="B19" s="30">
         <v>2.5</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="44" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="63">
+      <c r="E19" s="41">
         <v>44823</v>
       </c>
-      <c r="F19" s="63"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="30">
         <f t="shared" ref="G19" si="2">DAYS360(E19,F19)</f>
         <v>-44179</v>
       </c>
-      <c r="H19" s="64">
+      <c r="H19" s="42">
         <v>25</v>
       </c>
       <c r="I19" s="36"/>
@@ -2939,18 +2939,18 @@
       <c r="B20" s="30">
         <v>2.6</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="44" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="30">
         <v>0</v>
       </c>
-      <c r="H20" s="66"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="36"/>
       <c r="J20" s="37"/>
       <c r="K20" s="32"/>
@@ -3027,19 +3027,19 @@
       <c r="B21" s="30">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="44" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="30">
         <f>DAYS360(E21,F21)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="64"/>
+      <c r="H21" s="42"/>
       <c r="I21" s="36"/>
       <c r="J21" s="37"/>
       <c r="K21" s="32"/>
@@ -3116,17 +3116,17 @@
       <c r="B22" s="30">
         <v>2.7</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="44" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="30"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="30">
         <f t="shared" ref="G22:G23" si="3">DAYS360(E22,F22)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="66"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="36"/>
       <c r="J22" s="37"/>
       <c r="K22" s="32"/>
@@ -3203,15 +3203,15 @@
       <c r="B23" s="30">
         <v>2.8</v>
       </c>
-      <c r="C23" s="66"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="30"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H23" s="66"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="36"/>
       <c r="J23" s="37"/>
       <c r="K23" s="32"/>
@@ -3288,14 +3288,14 @@
       <c r="B24" s="30">
         <v>2.9</v>
       </c>
-      <c r="C24" s="66"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="30"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="30">
         <v>0</v>
       </c>
-      <c r="H24" s="66"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="36"/>
       <c r="J24" s="37"/>
       <c r="K24" s="32"/>
@@ -3372,19 +3372,19 @@
       <c r="B25" s="30">
         <v>2.4</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="44" t="s">
         <v>53</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="30">
         <f>DAYS360(E25,F25)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="64"/>
+      <c r="H25" s="42"/>
       <c r="I25" s="36"/>
       <c r="J25" s="37"/>
       <c r="K25" s="32"/>
@@ -3458,18 +3458,18 @@
     </row>
     <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
-      <c r="B26" s="67">
+      <c r="B26" s="45">
         <v>2.1</v>
       </c>
-      <c r="C26" s="66"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="30"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="30">
         <f>DAYS360(E26,F26)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="66"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="36"/>
       <c r="J26" s="37"/>
       <c r="K26" s="32"/>
@@ -3543,17 +3543,17 @@
     </row>
     <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
-      <c r="B27" s="67">
+      <c r="B27" s="45">
         <v>2.11</v>
       </c>
-      <c r="C27" s="66"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="30"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="30">
         <v>0</v>
       </c>
-      <c r="H27" s="66"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="36"/>
       <c r="J27" s="37"/>
       <c r="K27" s="32"/>
@@ -3627,17 +3627,17 @@
     </row>
     <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="62">
+      <c r="B28" s="40">
         <v>3</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
       <c r="I28" s="26"/>
       <c r="J28" s="27"/>
       <c r="K28" s="28"/>
@@ -3714,14 +3714,14 @@
       <c r="B29" s="30">
         <v>3.1</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="44" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="30">
         <f>DAYS360(E29,F29)</f>
         <v>0</v>
@@ -3803,14 +3803,14 @@
       <c r="B30" s="30">
         <v>3.2</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="44" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="30">
         <v>0</v>
       </c>
@@ -3891,20 +3891,20 @@
       <c r="B31" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="43" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="63">
+      <c r="E31" s="41">
         <v>44837</v>
       </c>
-      <c r="F31" s="63"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="30">
         <v>3</v>
       </c>
-      <c r="H31" s="64">
+      <c r="H31" s="42">
         <v>100</v>
       </c>
       <c r="I31" s="36"/>
@@ -3989,20 +3989,20 @@
       <c r="B32" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="43" t="s">
         <v>58</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="63">
+      <c r="E32" s="41">
         <v>44850</v>
       </c>
-      <c r="F32" s="63"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="30">
         <v>15</v>
       </c>
-      <c r="H32" s="64">
+      <c r="H32" s="42">
         <v>90</v>
       </c>
       <c r="I32" s="36"/>
@@ -4111,18 +4111,18 @@
       <c r="B33" s="30">
         <v>3.3</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="44" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="63">
+      <c r="E33" s="41">
         <v>44872</v>
       </c>
-      <c r="F33" s="63"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="30"/>
-      <c r="H33" s="64">
+      <c r="H33" s="42">
         <v>80</v>
       </c>
       <c r="I33" s="36"/>
@@ -4192,7 +4192,9 @@
       <c r="BS33" s="32"/>
       <c r="BT33" s="32"/>
       <c r="BU33" s="32"/>
-      <c r="BV33" s="32"/>
+      <c r="BV33" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="BW33" s="32"/>
       <c r="BX33" s="32"/>
       <c r="BY33" s="32"/>
@@ -4203,20 +4205,20 @@
       <c r="B34" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="44" t="s">
         <v>80</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="63">
+      <c r="E34" s="41">
         <v>44873</v>
       </c>
-      <c r="F34" s="63"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="30">
         <v>10</v>
       </c>
-      <c r="H34" s="64">
+      <c r="H34" s="42">
         <v>95</v>
       </c>
       <c r="I34" s="36"/>
@@ -4304,7 +4306,9 @@
       <c r="BU34" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="BV34" s="32"/>
+      <c r="BV34" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="BW34" s="32"/>
       <c r="BX34" s="32"/>
       <c r="BY34" s="32"/>
@@ -4312,20 +4316,20 @@
     </row>
     <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="44" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="63">
+      <c r="E35" s="41">
         <v>44854</v>
       </c>
-      <c r="F35" s="63"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="30">
         <v>9</v>
       </c>
-      <c r="H35" s="64">
+      <c r="H35" s="42">
         <v>90</v>
       </c>
       <c r="I35" s="36"/>
@@ -4411,7 +4415,9 @@
       <c r="BS35" s="32"/>
       <c r="BT35" s="32"/>
       <c r="BU35" s="32"/>
-      <c r="BV35" s="32"/>
+      <c r="BV35" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="BW35" s="32"/>
       <c r="BX35" s="32"/>
       <c r="BY35" s="32"/>
@@ -4420,20 +4426,20 @@
     <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="43" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="63">
+      <c r="E36" s="41">
         <v>44883</v>
       </c>
-      <c r="F36" s="63"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="30">
         <v>5</v>
       </c>
-      <c r="H36" s="64">
+      <c r="H36" s="42">
         <v>100</v>
       </c>
       <c r="I36" s="36"/>
@@ -4511,7 +4517,9 @@
       <c r="BS36" s="32"/>
       <c r="BT36" s="32"/>
       <c r="BU36" s="32"/>
-      <c r="BV36" s="32"/>
+      <c r="BV36" s="32" t="s">
+        <v>71</v>
+      </c>
       <c r="BW36" s="32"/>
       <c r="BX36" s="32"/>
       <c r="BY36" s="32"/>
@@ -4519,18 +4527,18 @@
     </row>
     <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
-      <c r="C37" s="66" t="s">
+      <c r="C37" s="44" t="s">
         <v>75</v>
       </c>
       <c r="D37" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="30">
         <v>0</v>
       </c>
-      <c r="H37" s="64">
+      <c r="H37" s="42">
         <v>100</v>
       </c>
       <c r="I37" s="36"/>
@@ -4606,18 +4614,18 @@
     </row>
     <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="44" t="s">
         <v>76</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="30">
         <v>0</v>
       </c>
-      <c r="H38" s="64">
+      <c r="H38" s="42">
         <v>100</v>
       </c>
       <c r="I38" s="36"/>
@@ -4694,19 +4702,19 @@
     <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="44" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
       <c r="G39" s="30">
         <f t="shared" ref="G39" si="4">DAYS360(E39,F39)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="64">
+      <c r="H39" s="42">
         <v>100</v>
       </c>
       <c r="I39" s="36"/>
@@ -4782,20 +4790,20 @@
     </row>
     <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="44" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="63">
+      <c r="E40" s="41">
         <v>44856</v>
       </c>
-      <c r="F40" s="63"/>
+      <c r="F40" s="41"/>
       <c r="G40" s="30">
         <v>0</v>
       </c>
-      <c r="H40" s="64">
+      <c r="H40" s="42">
         <v>75</v>
       </c>
       <c r="I40" s="36"/>
@@ -4896,18 +4904,18 @@
     <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="44" t="s">
         <v>65</v>
       </c>
       <c r="D41" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
       <c r="G41" s="30">
         <v>0</v>
       </c>
-      <c r="H41" s="64">
+      <c r="H41" s="42">
         <v>100</v>
       </c>
       <c r="I41" s="36"/>
@@ -5010,19 +5018,19 @@
     <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="44" t="s">
         <v>63</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
       <c r="G42" s="30">
         <f>DAYS360(E42,F42)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="64"/>
+      <c r="H42" s="42"/>
       <c r="I42" s="36"/>
       <c r="J42" s="37"/>
       <c r="K42" s="32"/>
@@ -5096,20 +5104,20 @@
     </row>
     <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="44" t="s">
         <v>68</v>
       </c>
       <c r="D43" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="63">
+      <c r="E43" s="41">
         <v>44859</v>
       </c>
-      <c r="F43" s="63"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="30">
         <v>0</v>
       </c>
-      <c r="H43" s="64">
+      <c r="H43" s="42">
         <v>5</v>
       </c>
       <c r="I43" s="36"/>
@@ -5184,17 +5192,17 @@
       <c r="BZ43" s="32"/>
     </row>
     <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="62">
+      <c r="B44" s="40">
         <v>4</v>
       </c>
-      <c r="C44" s="62" t="s">
+      <c r="C44" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
       <c r="I44" s="26"/>
       <c r="J44" s="27"/>
       <c r="K44" s="28"/>
@@ -5270,23 +5278,23 @@
       <c r="B45" s="30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="44" t="s">
         <v>72</v>
       </c>
       <c r="D45" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="63">
+      <c r="E45" s="41">
         <v>44823</v>
       </c>
-      <c r="F45" s="63">
+      <c r="F45" s="41">
         <v>44825</v>
       </c>
       <c r="G45" s="30">
         <f>DAYS360(E45,F45)</f>
         <v>2</v>
       </c>
-      <c r="H45" s="64">
+      <c r="H45" s="42">
         <v>100</v>
       </c>
       <c r="I45" s="36"/>
@@ -5368,10 +5376,10 @@
       <c r="B46" s="30">
         <v>4.2</v>
       </c>
-      <c r="C46" s="66"/>
+      <c r="C46" s="44"/>
       <c r="D46" s="30"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="30">
         <v>0</v>
       </c>
@@ -5451,10 +5459,10 @@
       <c r="B47" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="66"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="30"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="30">
         <f t="shared" ref="G47:G49" si="5">DAYS360(E47,F47)</f>
         <v>0</v>
@@ -5535,15 +5543,15 @@
       <c r="B48" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="66"/>
+      <c r="C48" s="44"/>
       <c r="D48" s="30"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
       <c r="G48" s="30">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H48" s="64"/>
+      <c r="H48" s="42"/>
       <c r="I48" s="36"/>
       <c r="J48" s="37"/>
       <c r="K48" s="32"/>
@@ -5619,10 +5627,10 @@
       <c r="B49" s="30">
         <v>4.3</v>
       </c>
-      <c r="C49" s="66"/>
+      <c r="C49" s="44"/>
       <c r="D49" s="30"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
       <c r="G49" s="30">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5703,10 +5711,10 @@
       <c r="B50" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="68"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="30"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
       <c r="G50" s="30">
         <v>0</v>
       </c>
@@ -5784,26 +5792,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5820,6 +5808,26 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H50">
     <cfRule type="colorScale" priority="18">
@@ -5847,12 +5855,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6085,15 +6090,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6118,18 +6135,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gantt Chart update and Puzzle doc
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33463DE-EB33-4634-8E04-756456C5BB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC06E47F-4021-4D45-A6E7-286A09FD5347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="83">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -153,9 +153,6 @@
     <t>W12 11/21/2022</t>
   </si>
   <si>
-    <t>W13 12/28/2022</t>
-  </si>
-  <si>
     <t>W14 12/5/2022</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>4.3.1</t>
   </si>
   <si>
-    <t>Landscape</t>
-  </si>
-  <si>
     <t>Setup</t>
   </si>
   <si>
@@ -210,9 +204,6 @@
     <t>Inventory</t>
   </si>
   <si>
-    <t>Narrative/Story</t>
-  </si>
-  <si>
     <t>BJ</t>
   </si>
   <si>
@@ -274,6 +265,21 @@
   </si>
   <si>
     <t>Snake Game</t>
+  </si>
+  <si>
+    <t>Hazard Light</t>
+  </si>
+  <si>
+    <t>Narrative/Story/Animations</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>W13 11/28/2022</t>
+  </si>
+  <si>
+    <t>Landscape/Planets</t>
   </si>
 </sst>
 </file>
@@ -789,6 +795,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -805,14 +840,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -824,30 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,22 +1175,22 @@
   </sheetPr>
   <dimension ref="A1:BZ50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="9" max="78" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1264,40 +1270,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="50"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1346,7 +1352,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1426,13 +1432,13 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="54"/>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="64" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="56"/>
@@ -1448,7 +1454,7 @@
       <c r="M4" s="54"/>
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
-      <c r="P4" s="57" t="s">
+      <c r="P4" s="65" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="56"/>
@@ -1514,13 +1520,13 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="54"/>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="56"/>
@@ -1536,7 +1542,7 @@
       <c r="M5" s="54"/>
       <c r="N5" s="54"/>
       <c r="O5" s="54"/>
-      <c r="P5" s="68">
+      <c r="P5" s="57">
         <v>44802</v>
       </c>
       <c r="Q5" s="56"/>
@@ -1602,10 +1608,10 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -1684,7 +1690,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1764,215 +1770,215 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="61"/>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="61"/>
-      <c r="AD8" s="61"/>
-      <c r="AE8" s="61"/>
-      <c r="AF8" s="61"/>
-      <c r="AG8" s="61"/>
-      <c r="AH8" s="61"/>
-      <c r="AI8" s="61"/>
-      <c r="AJ8" s="61"/>
-      <c r="AK8" s="61"/>
-      <c r="AL8" s="61"/>
-      <c r="AM8" s="62"/>
-      <c r="AN8" s="61"/>
-      <c r="AO8" s="61"/>
-      <c r="AP8" s="61"/>
-      <c r="AQ8" s="61"/>
-      <c r="AR8" s="61"/>
-      <c r="AS8" s="61"/>
-      <c r="AT8" s="61"/>
-      <c r="AU8" s="61"/>
-      <c r="AV8" s="61"/>
-      <c r="AW8" s="61"/>
-      <c r="AX8" s="61"/>
-      <c r="AY8" s="61"/>
-      <c r="AZ8" s="61"/>
-      <c r="BA8" s="61"/>
-      <c r="BB8" s="62"/>
-      <c r="BC8" s="61"/>
-      <c r="BD8" s="61"/>
-      <c r="BE8" s="61"/>
-      <c r="BF8" s="61"/>
-      <c r="BG8" s="61"/>
-      <c r="BH8" s="61"/>
-      <c r="BI8" s="61"/>
-      <c r="BJ8" s="61"/>
-      <c r="BK8" s="61"/>
-      <c r="BL8" s="61"/>
-      <c r="BM8" s="61"/>
-      <c r="BN8" s="61"/>
-      <c r="BO8" s="61"/>
-      <c r="BP8" s="61"/>
-      <c r="BQ8" s="61"/>
-      <c r="BR8" s="61"/>
-      <c r="BS8" s="61"/>
-      <c r="BT8" s="61"/>
-      <c r="BU8" s="61"/>
-      <c r="BV8" s="61"/>
-      <c r="BW8" s="61"/>
-      <c r="BX8" s="61"/>
-      <c r="BY8" s="61"/>
-      <c r="BZ8" s="66"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
+      <c r="AB8" s="48"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="48"/>
+      <c r="AE8" s="48"/>
+      <c r="AF8" s="48"/>
+      <c r="AG8" s="48"/>
+      <c r="AH8" s="48"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="48"/>
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="48"/>
+      <c r="AO8" s="48"/>
+      <c r="AP8" s="48"/>
+      <c r="AQ8" s="48"/>
+      <c r="AR8" s="48"/>
+      <c r="AS8" s="48"/>
+      <c r="AT8" s="48"/>
+      <c r="AU8" s="48"/>
+      <c r="AV8" s="48"/>
+      <c r="AW8" s="48"/>
+      <c r="AX8" s="48"/>
+      <c r="AY8" s="48"/>
+      <c r="AZ8" s="48"/>
+      <c r="BA8" s="48"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="48"/>
+      <c r="BD8" s="48"/>
+      <c r="BE8" s="48"/>
+      <c r="BF8" s="48"/>
+      <c r="BG8" s="48"/>
+      <c r="BH8" s="48"/>
+      <c r="BI8" s="48"/>
+      <c r="BJ8" s="48"/>
+      <c r="BK8" s="48"/>
+      <c r="BL8" s="48"/>
+      <c r="BM8" s="48"/>
+      <c r="BN8" s="48"/>
+      <c r="BO8" s="48"/>
+      <c r="BP8" s="48"/>
+      <c r="BQ8" s="48"/>
+      <c r="BR8" s="48"/>
+      <c r="BS8" s="48"/>
+      <c r="BT8" s="48"/>
+      <c r="BU8" s="48"/>
+      <c r="BV8" s="48"/>
+      <c r="BW8" s="48"/>
+      <c r="BX8" s="48"/>
+      <c r="BY8" s="48"/>
+      <c r="BZ8" s="49"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="63" t="s">
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="63" t="s">
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="63" t="s">
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="63" t="s">
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="63" t="s">
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="51"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="64"/>
-      <c r="AE9" s="64"/>
-      <c r="AF9" s="64"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="63" t="s">
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
+      <c r="AG9" s="52"/>
+      <c r="AH9" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="64"/>
-      <c r="AJ9" s="64"/>
-      <c r="AK9" s="64"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="63" t="s">
+      <c r="AI9" s="51"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="51"/>
+      <c r="AL9" s="52"/>
+      <c r="AM9" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="64"/>
-      <c r="AO9" s="64"/>
-      <c r="AP9" s="64"/>
-      <c r="AQ9" s="65"/>
-      <c r="AR9" s="63" t="s">
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="51"/>
+      <c r="AP9" s="51"/>
+      <c r="AQ9" s="52"/>
+      <c r="AR9" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="64"/>
-      <c r="AT9" s="64"/>
-      <c r="AU9" s="64"/>
-      <c r="AV9" s="65"/>
-      <c r="AW9" s="63" t="s">
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="51"/>
+      <c r="AU9" s="51"/>
+      <c r="AV9" s="52"/>
+      <c r="AW9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="64"/>
-      <c r="AY9" s="64"/>
-      <c r="AZ9" s="64"/>
-      <c r="BA9" s="65"/>
-      <c r="BB9" s="63" t="s">
+      <c r="AX9" s="51"/>
+      <c r="AY9" s="51"/>
+      <c r="AZ9" s="51"/>
+      <c r="BA9" s="52"/>
+      <c r="BB9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="64"/>
-      <c r="BD9" s="64"/>
-      <c r="BE9" s="64"/>
-      <c r="BF9" s="65"/>
-      <c r="BG9" s="63" t="s">
+      <c r="BC9" s="51"/>
+      <c r="BD9" s="51"/>
+      <c r="BE9" s="51"/>
+      <c r="BF9" s="52"/>
+      <c r="BG9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="64"/>
-      <c r="BI9" s="64"/>
-      <c r="BJ9" s="64"/>
-      <c r="BK9" s="65"/>
-      <c r="BL9" s="63" t="s">
+      <c r="BH9" s="51"/>
+      <c r="BI9" s="51"/>
+      <c r="BJ9" s="51"/>
+      <c r="BK9" s="52"/>
+      <c r="BL9" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="64"/>
-      <c r="BN9" s="64"/>
-      <c r="BO9" s="64"/>
-      <c r="BP9" s="65"/>
-      <c r="BQ9" s="63" t="s">
+      <c r="BM9" s="51"/>
+      <c r="BN9" s="51"/>
+      <c r="BO9" s="51"/>
+      <c r="BP9" s="52"/>
+      <c r="BQ9" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="BR9" s="51"/>
+      <c r="BS9" s="51"/>
+      <c r="BT9" s="51"/>
+      <c r="BU9" s="52"/>
+      <c r="BV9" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="BR9" s="64"/>
-      <c r="BS9" s="64"/>
-      <c r="BT9" s="64"/>
-      <c r="BU9" s="65"/>
-      <c r="BV9" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="BW9" s="64"/>
-      <c r="BX9" s="64"/>
-      <c r="BY9" s="64"/>
-      <c r="BZ9" s="65"/>
+      <c r="BW9" s="51"/>
+      <c r="BX9" s="51"/>
+      <c r="BY9" s="51"/>
+      <c r="BZ9" s="52"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="40">
         <v>1</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
@@ -2050,7 +2056,7 @@
       <c r="BY10" s="26"/>
       <c r="BZ10" s="26"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="30">
         <v>1.1000000000000001</v>
@@ -2145,7 +2151,7 @@
       <c r="BY11" s="32"/>
       <c r="BZ11" s="32"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
         <v>13</v>
@@ -2240,7 +2246,7 @@
       <c r="BY12" s="32"/>
       <c r="BZ12" s="32"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="30">
         <v>1.2</v>
@@ -2335,7 +2341,7 @@
       <c r="BY13" s="32"/>
       <c r="BZ13" s="32"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="30">
         <v>1.3</v>
@@ -2430,7 +2436,7 @@
       <c r="BY14" s="32"/>
       <c r="BZ14" s="32"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="40">
         <v>2</v>
@@ -2514,26 +2520,28 @@
       <c r="BY15" s="26"/>
       <c r="BZ15" s="26"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="30">
         <v>2.1</v>
       </c>
       <c r="C16" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="30" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="41">
         <v>44851</v>
       </c>
-      <c r="F16" s="41"/>
+      <c r="F16" s="41">
+        <v>44868</v>
+      </c>
       <c r="G16" s="30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H16" s="42">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I16" s="36"/>
       <c r="J16" s="37"/>
@@ -2566,19 +2574,19 @@
       <c r="AK16" s="39"/>
       <c r="AL16" s="39"/>
       <c r="AM16" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AN16" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AO16" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AP16" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AQ16" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AR16" s="34"/>
       <c r="AS16" s="34"/>
@@ -2586,9 +2594,15 @@
       <c r="AU16" s="34"/>
       <c r="AV16" s="34"/>
       <c r="AW16" s="32"/>
-      <c r="AX16" s="32"/>
-      <c r="AY16" s="32"/>
-      <c r="AZ16" s="32"/>
+      <c r="AX16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ16" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="BA16" s="32"/>
       <c r="BB16" s="32"/>
       <c r="BC16" s="32"/>
@@ -2616,27 +2630,29 @@
       <c r="BY16" s="32"/>
       <c r="BZ16" s="32"/>
     </row>
-    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="30">
         <v>2.2999999999999998</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" s="41">
         <v>44830</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="41">
+        <v>44875</v>
+      </c>
       <c r="G17" s="30">
         <f t="shared" ref="G17" si="1">DAYS360(E17,F17)</f>
-        <v>-44186</v>
+        <v>44</v>
       </c>
       <c r="H17" s="42">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I17" s="36"/>
       <c r="J17" s="37"/>
@@ -2654,28 +2670,28 @@
       <c r="V17" s="32"/>
       <c r="W17" s="32"/>
       <c r="X17" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Y17" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Z17" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AA17" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AB17" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AC17" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AD17" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AE17" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AF17" s="33"/>
       <c r="AG17" s="33"/>
@@ -2701,8 +2717,12 @@
       <c r="BA17" s="32"/>
       <c r="BB17" s="32"/>
       <c r="BC17" s="32"/>
-      <c r="BD17" s="32"/>
-      <c r="BE17" s="32"/>
+      <c r="BD17" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE17" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="BF17" s="32"/>
       <c r="BG17" s="35"/>
       <c r="BH17" s="35"/>
@@ -2725,26 +2745,28 @@
       <c r="BY17" s="32"/>
       <c r="BZ17" s="32"/>
     </row>
-    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" s="41">
         <v>44840</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="41">
+        <v>44846</v>
+      </c>
       <c r="G18" s="30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H18" s="42">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="I18" s="36"/>
       <c r="J18" s="37"/>
@@ -2770,25 +2792,25 @@
       <c r="AD18" s="33"/>
       <c r="AE18" s="33"/>
       <c r="AF18" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AG18" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AH18" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AI18" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AJ18" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AK18" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AL18" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AM18" s="39"/>
       <c r="AN18" s="39"/>
@@ -2831,27 +2853,29 @@
       <c r="BY18" s="32"/>
       <c r="BZ18" s="32"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29"/>
       <c r="B19" s="30">
         <v>2.5</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="41">
         <v>44823</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="41">
+        <v>44867</v>
+      </c>
       <c r="G19" s="30">
         <f t="shared" ref="G19" si="2">DAYS360(E19,F19)</f>
-        <v>-44179</v>
+        <v>43</v>
       </c>
       <c r="H19" s="42">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="I19" s="36"/>
       <c r="J19" s="37"/>
@@ -2864,19 +2888,19 @@
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
       <c r="S19" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T19" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="U19" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="V19" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="W19" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="X19" s="32"/>
       <c r="Y19" s="32"/>
@@ -2898,10 +2922,16 @@
       <c r="AO19" s="39"/>
       <c r="AP19" s="39"/>
       <c r="AQ19" s="39"/>
-      <c r="AR19" s="34"/>
-      <c r="AS19" s="34"/>
+      <c r="AR19" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS19" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="AT19" s="34"/>
-      <c r="AU19" s="34"/>
+      <c r="AU19" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="AV19" s="34"/>
       <c r="AW19" s="32"/>
       <c r="AX19" s="32"/>
@@ -2934,23 +2964,29 @@
       <c r="BY19" s="32"/>
       <c r="BZ19" s="32"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29"/>
       <c r="B20" s="30">
         <v>2.6</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="E20" s="41">
+        <v>44877</v>
+      </c>
+      <c r="F20" s="41">
+        <v>44898</v>
+      </c>
       <c r="G20" s="30">
-        <v>0</v>
-      </c>
-      <c r="H20" s="44"/>
+        <v>20</v>
+      </c>
+      <c r="H20" s="44">
+        <v>100</v>
+      </c>
       <c r="I20" s="36"/>
       <c r="J20" s="37"/>
       <c r="K20" s="32"/>
@@ -3002,36 +3038,62 @@
       <c r="BE20" s="32"/>
       <c r="BF20" s="32"/>
       <c r="BG20" s="35"/>
-      <c r="BH20" s="35"/>
+      <c r="BH20" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="BI20" s="35"/>
-      <c r="BJ20" s="35"/>
-      <c r="BK20" s="35"/>
-      <c r="BL20" s="32"/>
-      <c r="BM20" s="32"/>
-      <c r="BN20" s="32"/>
-      <c r="BO20" s="32"/>
-      <c r="BP20" s="32"/>
-      <c r="BQ20" s="32"/>
-      <c r="BR20" s="32"/>
-      <c r="BS20" s="32"/>
-      <c r="BT20" s="32"/>
-      <c r="BU20" s="32"/>
+      <c r="BJ20" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK20" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="BL20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BN20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BQ20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BS20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BT20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BU20" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="BV20" s="32"/>
       <c r="BW20" s="32"/>
       <c r="BX20" s="32"/>
       <c r="BY20" s="32"/>
       <c r="BZ20" s="32"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="29"/>
       <c r="B21" s="30">
         <v>2.2000000000000002</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
@@ -3111,13 +3173,13 @@
       <c r="BY21" s="32"/>
       <c r="BZ21" s="32"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="30">
         <v>2.7</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="41"/>
@@ -3198,7 +3260,7 @@
       <c r="BY22" s="32"/>
       <c r="BZ22" s="32"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="30">
         <v>2.8</v>
@@ -3283,7 +3345,7 @@
       <c r="BY23" s="32"/>
       <c r="BZ23" s="32"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="30">
         <v>2.9</v>
@@ -3367,16 +3429,16 @@
       <c r="BY24" s="32"/>
       <c r="BZ24" s="32"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="30">
         <v>2.4</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
@@ -3456,7 +3518,7 @@
       <c r="BY25" s="32"/>
       <c r="BZ25" s="32"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29"/>
       <c r="B26" s="45">
         <v>2.1</v>
@@ -3541,7 +3603,7 @@
       <c r="BY26" s="32"/>
       <c r="BZ26" s="32"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="45">
         <v>2.11</v>
@@ -3625,7 +3687,7 @@
       <c r="BY27" s="32"/>
       <c r="BZ27" s="32"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="40">
         <v>3</v>
@@ -3709,16 +3771,16 @@
       <c r="BY28" s="26"/>
       <c r="BZ28" s="26"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
       <c r="B29" s="30">
         <v>3.1</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -3798,16 +3860,16 @@
       <c r="BY29" s="32"/>
       <c r="BZ29" s="32"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29"/>
       <c r="B30" s="30">
         <v>3.2</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
@@ -3886,16 +3948,16 @@
       <c r="BY30" s="32"/>
       <c r="BZ30" s="32"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
       <c r="B31" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E31" s="41">
         <v>44837</v>
@@ -3928,15 +3990,15 @@
       <c r="AA31" s="32"/>
       <c r="AB31" s="32"/>
       <c r="AC31" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AD31" s="33"/>
       <c r="AE31" s="33"/>
       <c r="AF31" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AG31" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AH31" s="32"/>
       <c r="AI31" s="32"/>
@@ -3984,16 +4046,16 @@
       <c r="BY31" s="32"/>
       <c r="BZ31" s="32"/>
     </row>
-    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
       <c r="B32" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E32" s="41">
         <v>44850</v>
@@ -4033,29 +4095,29 @@
       <c r="AH32" s="32"/>
       <c r="AI32" s="32"/>
       <c r="AJ32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AK32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AL32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AM32" s="32"/>
       <c r="AN32" s="32"/>
       <c r="AO32" s="32"/>
       <c r="AP32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AQ32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AR32" s="34"/>
       <c r="AS32" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AT32" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AU32" s="34"/>
       <c r="AV32" s="34"/>
@@ -4064,16 +4126,16 @@
       <c r="AY32" s="32"/>
       <c r="AZ32" s="32"/>
       <c r="BA32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BB32" s="32"/>
       <c r="BC32" s="32"/>
       <c r="BD32" s="32"/>
       <c r="BE32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BF32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BG32" s="35"/>
       <c r="BH32" s="35"/>
@@ -4089,33 +4151,33 @@
       <c r="BR32" s="32"/>
       <c r="BS32" s="32"/>
       <c r="BT32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BU32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BV32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BW32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BX32" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BY32" s="32"/>
       <c r="BZ32" s="32"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
       <c r="B33" s="30">
         <v>3.3</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E33" s="41">
         <v>44872</v>
@@ -4171,7 +4233,7 @@
       <c r="AZ33" s="32"/>
       <c r="BA33" s="32"/>
       <c r="BB33" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BC33" s="32"/>
       <c r="BD33" s="32"/>
@@ -4193,23 +4255,23 @@
       <c r="BT33" s="32"/>
       <c r="BU33" s="32"/>
       <c r="BV33" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BW33" s="32"/>
       <c r="BX33" s="32"/>
       <c r="BY33" s="32"/>
       <c r="BZ33" s="32"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" s="41">
         <v>44873</v>
@@ -4269,58 +4331,58 @@
       <c r="BB34" s="32"/>
       <c r="BC34" s="32"/>
       <c r="BD34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BE34" s="32"/>
       <c r="BF34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BG34" s="35"/>
       <c r="BH34" s="35"/>
       <c r="BI34" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BJ34" s="35"/>
       <c r="BK34" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BL34" s="32"/>
       <c r="BM34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BN34" s="32"/>
       <c r="BO34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BP34" s="32"/>
       <c r="BQ34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BR34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BS34" s="32"/>
       <c r="BT34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BU34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BV34" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BW34" s="32"/>
       <c r="BX34" s="32"/>
       <c r="BY34" s="32"/>
       <c r="BZ34" s="32"/>
     </row>
-    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="30"/>
       <c r="C35" s="44" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E35" s="41">
         <v>44854</v>
@@ -4366,15 +4428,15 @@
       <c r="AN35" s="32"/>
       <c r="AO35" s="32"/>
       <c r="AP35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AQ35" s="32"/>
       <c r="AR35" s="34"/>
       <c r="AS35" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AT35" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AU35" s="34"/>
       <c r="AV35" s="34"/>
@@ -4383,13 +4445,13 @@
       <c r="AY35" s="32"/>
       <c r="AZ35" s="32"/>
       <c r="BA35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BB35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BC35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BD35" s="32"/>
       <c r="BE35" s="32"/>
@@ -4403,34 +4465,34 @@
       <c r="BM35" s="32"/>
       <c r="BN35" s="32"/>
       <c r="BO35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BP35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BQ35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BR35" s="32"/>
       <c r="BS35" s="32"/>
       <c r="BT35" s="32"/>
       <c r="BU35" s="32"/>
       <c r="BV35" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BW35" s="32"/>
       <c r="BX35" s="32"/>
       <c r="BY35" s="32"/>
       <c r="BZ35" s="32"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36" s="41">
         <v>44883</v>
@@ -4497,41 +4559,41 @@
       <c r="BI36" s="35"/>
       <c r="BJ36" s="35"/>
       <c r="BK36" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BL36" s="32"/>
       <c r="BM36" s="32"/>
       <c r="BN36" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BO36" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BP36" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BQ36" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BR36" s="32"/>
       <c r="BS36" s="32"/>
       <c r="BT36" s="32"/>
       <c r="BU36" s="32"/>
       <c r="BV36" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BW36" s="32"/>
       <c r="BX36" s="32"/>
       <c r="BY36" s="32"/>
       <c r="BZ36" s="32"/>
     </row>
-    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="30"/>
       <c r="C37" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="41"/>
@@ -4612,13 +4674,13 @@
       <c r="BY37" s="32"/>
       <c r="BZ37" s="32"/>
     </row>
-    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="30"/>
       <c r="C38" s="44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="41"/>
@@ -4699,14 +4761,14 @@
       <c r="BY38" s="32"/>
       <c r="BZ38" s="32"/>
     </row>
-    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="41"/>
@@ -4788,13 +4850,13 @@
       <c r="BY39" s="32"/>
       <c r="BZ39" s="32"/>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="30"/>
       <c r="C40" s="44" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E40" s="41">
         <v>44856</v>
@@ -4840,55 +4902,55 @@
       <c r="AN40" s="32"/>
       <c r="AO40" s="32"/>
       <c r="AP40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AQ40" s="32"/>
       <c r="AR40" s="34"/>
       <c r="AS40" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AT40" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AU40" s="34"/>
       <c r="AV40" s="34"/>
       <c r="AW40" s="32"/>
       <c r="AX40" s="32"/>
       <c r="AY40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AZ40" s="32"/>
       <c r="BA40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BB40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BC40" s="32"/>
       <c r="BD40" s="32"/>
       <c r="BE40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BF40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BG40" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BH40" s="35"/>
       <c r="BI40" s="35"/>
       <c r="BJ40" s="35"/>
       <c r="BK40" s="35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BL40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BM40" s="32"/>
       <c r="BN40" s="32"/>
       <c r="BO40" s="32"/>
       <c r="BP40" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BQ40" s="32"/>
       <c r="BR40" s="32"/>
@@ -4901,14 +4963,14 @@
       <c r="BY40" s="32"/>
       <c r="BZ40" s="32"/>
     </row>
-    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="41"/>
@@ -4941,57 +5003,57 @@
       <c r="AC41" s="33"/>
       <c r="AD41" s="33"/>
       <c r="AE41" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AF41" s="33"/>
       <c r="AG41" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AH41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AI41" s="32"/>
       <c r="AJ41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AK41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AL41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AM41" s="32"/>
       <c r="AN41" s="32"/>
       <c r="AO41" s="32"/>
       <c r="AP41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AQ41" s="32"/>
       <c r="AR41" s="34"/>
       <c r="AS41" s="34"/>
       <c r="AT41" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AU41" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AV41" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AW41" s="32"/>
       <c r="AX41" s="32"/>
       <c r="AY41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AZ41" s="32"/>
       <c r="BA41" s="32"/>
       <c r="BB41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BC41" s="32"/>
       <c r="BD41" s="32"/>
       <c r="BE41" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="BF41" s="32"/>
       <c r="BG41" s="35"/>
@@ -5015,14 +5077,14 @@
       <c r="BY41" s="32"/>
       <c r="BZ41" s="32"/>
     </row>
-    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="44" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E42" s="41"/>
       <c r="F42" s="41"/>
@@ -5102,13 +5164,13 @@
       <c r="BY42" s="32"/>
       <c r="BZ42" s="32"/>
     </row>
-    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="30"/>
       <c r="C43" s="44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E43" s="41">
         <v>44859</v>
@@ -5191,7 +5253,7 @@
       <c r="BY43" s="32"/>
       <c r="BZ43" s="32"/>
     </row>
-    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="40">
         <v>4</v>
       </c>
@@ -5274,15 +5336,15 @@
       <c r="BY44" s="26"/>
       <c r="BZ44" s="26"/>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="30">
         <v>4.0999999999999996</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E45" s="41">
         <v>44823</v>
@@ -5308,10 +5370,10 @@
       <c r="Q45" s="38"/>
       <c r="R45" s="38"/>
       <c r="S45" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T45" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="U45" s="32"/>
       <c r="V45" s="32"/>
@@ -5372,18 +5434,28 @@
       <c r="BY45" s="32"/>
       <c r="BZ45" s="32"/>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="30">
         <v>4.2</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
+      <c r="C46" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="41">
+        <v>44874</v>
+      </c>
+      <c r="F46" s="41">
+        <v>44876</v>
+      </c>
       <c r="G46" s="30">
-        <v>0</v>
-      </c>
-      <c r="H46" s="31"/>
+        <v>2</v>
+      </c>
+      <c r="H46" s="42">
+        <v>100</v>
+      </c>
       <c r="I46" s="36"/>
       <c r="J46" s="37"/>
       <c r="K46" s="32"/>
@@ -5432,8 +5504,12 @@
       <c r="BB46" s="32"/>
       <c r="BC46" s="32"/>
       <c r="BD46" s="32"/>
-      <c r="BE46" s="32"/>
-      <c r="BF46" s="32"/>
+      <c r="BE46" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF46" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="BG46" s="35"/>
       <c r="BH46" s="35"/>
       <c r="BI46" s="35"/>
@@ -5455,9 +5531,9 @@
       <c r="BY46" s="32"/>
       <c r="BZ46" s="32"/>
     </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="44"/>
       <c r="D47" s="30"/>
@@ -5539,9 +5615,9 @@
       <c r="BY47" s="32"/>
       <c r="BZ47" s="32"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="44"/>
       <c r="D48" s="30"/>
@@ -5623,7 +5699,7 @@
       <c r="BY48" s="32"/>
       <c r="BZ48" s="32"/>
     </row>
-    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="30">
         <v>4.3</v>
       </c>
@@ -5707,9 +5783,9 @@
       <c r="BY49" s="32"/>
       <c r="BZ49" s="32"/>
     </row>
-    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="46"/>
       <c r="D50" s="30"/>
@@ -5792,6 +5868,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5808,26 +5904,6 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H50">
     <cfRule type="colorScale" priority="18">
@@ -5855,9 +5931,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6090,27 +6169,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6135,9 +6202,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
*CHANGES TO GANTT CHART* Updating gantt chart
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UE_4.27\MoonGame\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C1EC9C-EDEA-4151-8B0E-2D0160AC17F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BCCA0-E4FC-45AB-A1B2-93BFD6B5270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="85">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Landscape/Planets</t>
+  </si>
+  <si>
+    <t>Interaction Interface</t>
+  </si>
+  <si>
+    <t>Get Rubiks Cube with Gun Puzzle</t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -657,11 +663,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -795,6 +812,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -811,14 +857,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -831,29 +872,8 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,24 +1193,24 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BZ50"/>
+  <dimension ref="A1:BZ52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="9" max="78" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="78" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1270,40 +1290,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="50"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1352,7 +1372,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1432,13 +1452,13 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="54"/>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="64" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="56"/>
@@ -1454,7 +1474,7 @@
       <c r="M4" s="54"/>
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
-      <c r="P4" s="57" t="s">
+      <c r="P4" s="65" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="56"/>
@@ -1520,13 +1540,13 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="54"/>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="56"/>
@@ -1542,7 +1562,7 @@
       <c r="M5" s="54"/>
       <c r="N5" s="54"/>
       <c r="O5" s="54"/>
-      <c r="P5" s="68">
+      <c r="P5" s="57">
         <v>44802</v>
       </c>
       <c r="Q5" s="56"/>
@@ -1608,7 +1628,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
         <v>46</v>
@@ -1690,7 +1710,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1770,209 +1790,209 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="61"/>
-      <c r="S8" s="61"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="61"/>
-      <c r="AD8" s="61"/>
-      <c r="AE8" s="61"/>
-      <c r="AF8" s="61"/>
-      <c r="AG8" s="61"/>
-      <c r="AH8" s="61"/>
-      <c r="AI8" s="61"/>
-      <c r="AJ8" s="61"/>
-      <c r="AK8" s="61"/>
-      <c r="AL8" s="61"/>
-      <c r="AM8" s="62"/>
-      <c r="AN8" s="61"/>
-      <c r="AO8" s="61"/>
-      <c r="AP8" s="61"/>
-      <c r="AQ8" s="61"/>
-      <c r="AR8" s="61"/>
-      <c r="AS8" s="61"/>
-      <c r="AT8" s="61"/>
-      <c r="AU8" s="61"/>
-      <c r="AV8" s="61"/>
-      <c r="AW8" s="61"/>
-      <c r="AX8" s="61"/>
-      <c r="AY8" s="61"/>
-      <c r="AZ8" s="61"/>
-      <c r="BA8" s="61"/>
-      <c r="BB8" s="62"/>
-      <c r="BC8" s="61"/>
-      <c r="BD8" s="61"/>
-      <c r="BE8" s="61"/>
-      <c r="BF8" s="61"/>
-      <c r="BG8" s="61"/>
-      <c r="BH8" s="61"/>
-      <c r="BI8" s="61"/>
-      <c r="BJ8" s="61"/>
-      <c r="BK8" s="61"/>
-      <c r="BL8" s="61"/>
-      <c r="BM8" s="61"/>
-      <c r="BN8" s="61"/>
-      <c r="BO8" s="61"/>
-      <c r="BP8" s="61"/>
-      <c r="BQ8" s="61"/>
-      <c r="BR8" s="61"/>
-      <c r="BS8" s="61"/>
-      <c r="BT8" s="61"/>
-      <c r="BU8" s="61"/>
-      <c r="BV8" s="61"/>
-      <c r="BW8" s="61"/>
-      <c r="BX8" s="61"/>
-      <c r="BY8" s="61"/>
-      <c r="BZ8" s="66"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
+      <c r="AB8" s="48"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="48"/>
+      <c r="AE8" s="48"/>
+      <c r="AF8" s="48"/>
+      <c r="AG8" s="48"/>
+      <c r="AH8" s="48"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="48"/>
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="48"/>
+      <c r="AO8" s="48"/>
+      <c r="AP8" s="48"/>
+      <c r="AQ8" s="48"/>
+      <c r="AR8" s="48"/>
+      <c r="AS8" s="48"/>
+      <c r="AT8" s="48"/>
+      <c r="AU8" s="48"/>
+      <c r="AV8" s="48"/>
+      <c r="AW8" s="48"/>
+      <c r="AX8" s="48"/>
+      <c r="AY8" s="48"/>
+      <c r="AZ8" s="48"/>
+      <c r="BA8" s="48"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="48"/>
+      <c r="BD8" s="48"/>
+      <c r="BE8" s="48"/>
+      <c r="BF8" s="48"/>
+      <c r="BG8" s="48"/>
+      <c r="BH8" s="48"/>
+      <c r="BI8" s="48"/>
+      <c r="BJ8" s="48"/>
+      <c r="BK8" s="48"/>
+      <c r="BL8" s="48"/>
+      <c r="BM8" s="48"/>
+      <c r="BN8" s="48"/>
+      <c r="BO8" s="48"/>
+      <c r="BP8" s="48"/>
+      <c r="BQ8" s="48"/>
+      <c r="BR8" s="48"/>
+      <c r="BS8" s="48"/>
+      <c r="BT8" s="48"/>
+      <c r="BU8" s="48"/>
+      <c r="BV8" s="48"/>
+      <c r="BW8" s="48"/>
+      <c r="BX8" s="48"/>
+      <c r="BY8" s="48"/>
+      <c r="BZ8" s="49"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="63" t="s">
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="63" t="s">
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="63" t="s">
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="63" t="s">
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="63" t="s">
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="51"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="64"/>
-      <c r="AE9" s="64"/>
-      <c r="AF9" s="64"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="63" t="s">
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
+      <c r="AG9" s="52"/>
+      <c r="AH9" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="64"/>
-      <c r="AJ9" s="64"/>
-      <c r="AK9" s="64"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="63" t="s">
+      <c r="AI9" s="51"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="51"/>
+      <c r="AL9" s="52"/>
+      <c r="AM9" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="64"/>
-      <c r="AO9" s="64"/>
-      <c r="AP9" s="64"/>
-      <c r="AQ9" s="65"/>
-      <c r="AR9" s="63" t="s">
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="51"/>
+      <c r="AP9" s="51"/>
+      <c r="AQ9" s="52"/>
+      <c r="AR9" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="64"/>
-      <c r="AT9" s="64"/>
-      <c r="AU9" s="64"/>
-      <c r="AV9" s="65"/>
-      <c r="AW9" s="63" t="s">
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="51"/>
+      <c r="AU9" s="51"/>
+      <c r="AV9" s="52"/>
+      <c r="AW9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="64"/>
-      <c r="AY9" s="64"/>
-      <c r="AZ9" s="64"/>
-      <c r="BA9" s="65"/>
-      <c r="BB9" s="63" t="s">
+      <c r="AX9" s="51"/>
+      <c r="AY9" s="51"/>
+      <c r="AZ9" s="51"/>
+      <c r="BA9" s="52"/>
+      <c r="BB9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="64"/>
-      <c r="BD9" s="64"/>
-      <c r="BE9" s="64"/>
-      <c r="BF9" s="65"/>
-      <c r="BG9" s="63" t="s">
+      <c r="BC9" s="51"/>
+      <c r="BD9" s="51"/>
+      <c r="BE9" s="51"/>
+      <c r="BF9" s="52"/>
+      <c r="BG9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="64"/>
-      <c r="BI9" s="64"/>
-      <c r="BJ9" s="64"/>
-      <c r="BK9" s="65"/>
-      <c r="BL9" s="63" t="s">
+      <c r="BH9" s="51"/>
+      <c r="BI9" s="51"/>
+      <c r="BJ9" s="51"/>
+      <c r="BK9" s="52"/>
+      <c r="BL9" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="64"/>
-      <c r="BN9" s="64"/>
-      <c r="BO9" s="64"/>
-      <c r="BP9" s="65"/>
-      <c r="BQ9" s="63" t="s">
+      <c r="BM9" s="51"/>
+      <c r="BN9" s="51"/>
+      <c r="BO9" s="51"/>
+      <c r="BP9" s="52"/>
+      <c r="BQ9" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="BR9" s="64"/>
-      <c r="BS9" s="64"/>
-      <c r="BT9" s="64"/>
-      <c r="BU9" s="65"/>
-      <c r="BV9" s="63" t="s">
+      <c r="BR9" s="51"/>
+      <c r="BS9" s="51"/>
+      <c r="BT9" s="51"/>
+      <c r="BU9" s="52"/>
+      <c r="BV9" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="BW9" s="64"/>
-      <c r="BX9" s="64"/>
-      <c r="BY9" s="64"/>
-      <c r="BZ9" s="65"/>
+      <c r="BW9" s="51"/>
+      <c r="BX9" s="51"/>
+      <c r="BY9" s="51"/>
+      <c r="BZ9" s="52"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="40">
         <v>1</v>
@@ -2056,7 +2076,7 @@
       <c r="BY10" s="26"/>
       <c r="BZ10" s="26"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="30">
         <v>1.1000000000000001</v>
@@ -2151,7 +2171,7 @@
       <c r="BY11" s="32"/>
       <c r="BZ11" s="32"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
         <v>13</v>
@@ -2246,7 +2266,7 @@
       <c r="BY12" s="32"/>
       <c r="BZ12" s="32"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="30">
         <v>1.2</v>
@@ -2341,7 +2361,7 @@
       <c r="BY13" s="32"/>
       <c r="BZ13" s="32"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="30">
         <v>1.3</v>
@@ -2436,7 +2456,7 @@
       <c r="BY14" s="32"/>
       <c r="BZ14" s="32"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="40">
         <v>2</v>
@@ -2520,7 +2540,7 @@
       <c r="BY15" s="26"/>
       <c r="BZ15" s="26"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="30">
         <v>2.1</v>
@@ -2630,7 +2650,7 @@
       <c r="BY16" s="32"/>
       <c r="BZ16" s="32"/>
     </row>
-    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="30">
         <v>2.2999999999999998</v>
@@ -2745,7 +2765,7 @@
       <c r="BY17" s="32"/>
       <c r="BZ17" s="32"/>
     </row>
-    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
@@ -2853,7 +2873,7 @@
       <c r="BY18" s="32"/>
       <c r="BZ18" s="32"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29"/>
       <c r="B19" s="30">
         <v>2.5</v>
@@ -2964,7 +2984,7 @@
       <c r="BY19" s="32"/>
       <c r="BZ19" s="32"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29"/>
       <c r="B20" s="30">
         <v>2.6</v>
@@ -3084,7 +3104,7 @@
       <c r="BY20" s="32"/>
       <c r="BZ20" s="32"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="29"/>
       <c r="B21" s="30">
         <v>2.2000000000000002</v>
@@ -3173,7 +3193,7 @@
       <c r="BY21" s="32"/>
       <c r="BZ21" s="32"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="30">
         <v>2.7</v>
@@ -3260,7 +3280,7 @@
       <c r="BY22" s="32"/>
       <c r="BZ22" s="32"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="30">
         <v>2.8</v>
@@ -3345,7 +3365,7 @@
       <c r="BY23" s="32"/>
       <c r="BZ23" s="32"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="30">
         <v>2.9</v>
@@ -3429,7 +3449,7 @@
       <c r="BY24" s="32"/>
       <c r="BZ24" s="32"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="30">
         <v>2.4</v>
@@ -3518,7 +3538,7 @@
       <c r="BY25" s="32"/>
       <c r="BZ25" s="32"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29"/>
       <c r="B26" s="45">
         <v>2.1</v>
@@ -3603,7 +3623,7 @@
       <c r="BY26" s="32"/>
       <c r="BZ26" s="32"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="45">
         <v>2.11</v>
@@ -3687,7 +3707,7 @@
       <c r="BY27" s="32"/>
       <c r="BZ27" s="32"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="40">
         <v>3</v>
@@ -3771,7 +3791,7 @@
       <c r="BY28" s="26"/>
       <c r="BZ28" s="26"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
       <c r="B29" s="30">
         <v>3.1</v>
@@ -3860,7 +3880,7 @@
       <c r="BY29" s="32"/>
       <c r="BZ29" s="32"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29"/>
       <c r="B30" s="30">
         <v>3.2</v>
@@ -3948,7 +3968,7 @@
       <c r="BY30" s="32"/>
       <c r="BZ30" s="32"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
       <c r="B31" s="30" t="s">
         <v>17</v>
@@ -4050,7 +4070,7 @@
       <c r="BY31" s="32"/>
       <c r="BZ31" s="32"/>
     </row>
-    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
       <c r="B32" s="30" t="s">
         <v>18</v>
@@ -4172,7 +4192,7 @@
       <c r="BY32" s="32"/>
       <c r="BZ32" s="32"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
       <c r="B33" s="30">
         <v>3.3</v>
@@ -4272,7 +4292,7 @@
       <c r="BY33" s="32"/>
       <c r="BZ33" s="32"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="30" t="s">
         <v>19</v>
@@ -4392,7 +4412,7 @@
       <c r="BY34" s="32"/>
       <c r="BZ34" s="32"/>
     </row>
-    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="30"/>
       <c r="C35" s="44" t="s">
         <v>67</v>
@@ -4507,7 +4527,7 @@
       <c r="BY35" s="32"/>
       <c r="BZ35" s="32"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="43" t="s">
@@ -4609,7 +4629,7 @@
       <c r="BY36" s="32"/>
       <c r="BZ36" s="32"/>
     </row>
-    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="30"/>
       <c r="C37" s="44" t="s">
         <v>72</v>
@@ -4617,8 +4637,12 @@
       <c r="D37" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="41">
+        <v>44875</v>
+      </c>
+      <c r="F37" s="41">
+        <v>44878</v>
+      </c>
       <c r="G37" s="30">
         <v>0</v>
       </c>
@@ -4671,11 +4695,21 @@
       <c r="AZ37" s="32"/>
       <c r="BA37" s="32"/>
       <c r="BB37" s="32"/>
-      <c r="BC37" s="32"/>
-      <c r="BD37" s="32"/>
-      <c r="BE37" s="32"/>
-      <c r="BF37" s="32"/>
-      <c r="BG37" s="35"/>
+      <c r="BC37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BD37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BE37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BF37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG37" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="BH37" s="35"/>
       <c r="BI37" s="35"/>
       <c r="BJ37" s="35"/>
@@ -4686,17 +4720,35 @@
       <c r="BO37" s="32"/>
       <c r="BP37" s="32"/>
       <c r="BQ37" s="32"/>
-      <c r="BR37" s="32"/>
-      <c r="BS37" s="32"/>
-      <c r="BT37" s="32"/>
-      <c r="BU37" s="32"/>
-      <c r="BV37" s="32"/>
-      <c r="BW37" s="32"/>
-      <c r="BX37" s="32"/>
-      <c r="BY37" s="32"/>
-      <c r="BZ37" s="32"/>
+      <c r="BR37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BX37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BY37" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BZ37" s="32" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="30"/>
       <c r="C38" s="44" t="s">
         <v>73</v>
@@ -4704,8 +4756,12 @@
       <c r="D38" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
+      <c r="E38" s="41">
+        <v>44880</v>
+      </c>
+      <c r="F38" s="41">
+        <v>44886</v>
+      </c>
       <c r="G38" s="30">
         <v>0</v>
       </c>
@@ -4763,27 +4819,53 @@
       <c r="BE38" s="32"/>
       <c r="BF38" s="32"/>
       <c r="BG38" s="35"/>
-      <c r="BH38" s="35"/>
-      <c r="BI38" s="35"/>
-      <c r="BJ38" s="35"/>
-      <c r="BK38" s="35"/>
+      <c r="BH38" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI38" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="BJ38" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="BK38" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="BL38" s="32"/>
       <c r="BM38" s="32"/>
       <c r="BN38" s="32"/>
       <c r="BO38" s="32"/>
       <c r="BP38" s="32"/>
       <c r="BQ38" s="32"/>
-      <c r="BR38" s="32"/>
-      <c r="BS38" s="32"/>
-      <c r="BT38" s="32"/>
-      <c r="BU38" s="32"/>
-      <c r="BV38" s="32"/>
-      <c r="BW38" s="32"/>
-      <c r="BX38" s="32"/>
-      <c r="BY38" s="32"/>
-      <c r="BZ38" s="32"/>
+      <c r="BR38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BX38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BY38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BZ38" s="32" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="44" t="s">
@@ -4792,11 +4874,15 @@
       <c r="D39" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
+      <c r="E39" s="41">
+        <v>44824</v>
+      </c>
+      <c r="F39" s="41">
+        <v>44872</v>
+      </c>
       <c r="G39" s="30">
         <f t="shared" ref="G39" si="4">DAYS360(E39,F39)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H39" s="42">
         <v>100</v>
@@ -4816,24 +4902,50 @@
       <c r="U39" s="32"/>
       <c r="V39" s="32"/>
       <c r="W39" s="32"/>
-      <c r="X39" s="32"/>
-      <c r="Y39" s="32"/>
-      <c r="Z39" s="32"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="32"/>
-      <c r="AC39" s="33"/>
+      <c r="X39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC39" s="33" t="s">
+        <v>68</v>
+      </c>
       <c r="AD39" s="33"/>
       <c r="AE39" s="33"/>
       <c r="AF39" s="33"/>
       <c r="AG39" s="33"/>
       <c r="AH39" s="32"/>
-      <c r="AI39" s="32"/>
-      <c r="AJ39" s="32"/>
-      <c r="AK39" s="32"/>
-      <c r="AL39" s="32"/>
-      <c r="AM39" s="32"/>
-      <c r="AN39" s="32"/>
-      <c r="AO39" s="32"/>
+      <c r="AI39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO39" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="AP39" s="32"/>
       <c r="AQ39" s="32"/>
       <c r="AR39" s="34"/>
@@ -4841,10 +4953,18 @@
       <c r="AT39" s="34"/>
       <c r="AU39" s="34"/>
       <c r="AV39" s="34"/>
-      <c r="AW39" s="32"/>
-      <c r="AX39" s="32"/>
-      <c r="AY39" s="32"/>
-      <c r="AZ39" s="32"/>
+      <c r="AW39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ39" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BA39" s="32"/>
       <c r="BB39" s="32"/>
       <c r="BC39" s="32"/>
@@ -4860,19 +4980,41 @@
       <c r="BM39" s="32"/>
       <c r="BN39" s="32"/>
       <c r="BO39" s="32"/>
-      <c r="BP39" s="32"/>
-      <c r="BQ39" s="32"/>
-      <c r="BR39" s="32"/>
-      <c r="BS39" s="32"/>
-      <c r="BT39" s="32"/>
-      <c r="BU39" s="32"/>
-      <c r="BV39" s="32"/>
-      <c r="BW39" s="32"/>
-      <c r="BX39" s="32"/>
-      <c r="BY39" s="32"/>
-      <c r="BZ39" s="32"/>
+      <c r="BP39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BQ39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BX39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BY39" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BZ39" s="32" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="30"/>
       <c r="C40" s="44" t="s">
         <v>66</v>
@@ -4985,7 +5127,7 @@
       <c r="BY40" s="32"/>
       <c r="BZ40" s="32"/>
     </row>
-    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="44" t="s">
@@ -5099,7 +5241,7 @@
       <c r="BY41" s="32"/>
       <c r="BZ41" s="32"/>
     </row>
-    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="44" t="s">
@@ -5186,7 +5328,7 @@
       <c r="BY42" s="32"/>
       <c r="BZ42" s="32"/>
     </row>
-    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="30"/>
       <c r="C43" s="44" t="s">
         <v>65</v>
@@ -5275,109 +5417,122 @@
       <c r="BY43" s="32"/>
       <c r="BZ43" s="32"/>
     </row>
-    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="40">
-        <v>4</v>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
-      <c r="Q44" s="26"/>
-      <c r="R44" s="26"/>
-      <c r="S44" s="26"/>
-      <c r="T44" s="26"/>
-      <c r="U44" s="26"/>
-      <c r="V44" s="26"/>
-      <c r="W44" s="26"/>
-      <c r="X44" s="26"/>
-      <c r="Y44" s="26"/>
-      <c r="Z44" s="26"/>
-      <c r="AA44" s="26"/>
-      <c r="AB44" s="26"/>
-      <c r="AC44" s="26"/>
-      <c r="AD44" s="26"/>
-      <c r="AE44" s="26"/>
-      <c r="AF44" s="26"/>
-      <c r="AG44" s="26"/>
-      <c r="AH44" s="26"/>
-      <c r="AI44" s="26"/>
-      <c r="AJ44" s="26"/>
-      <c r="AK44" s="26"/>
-      <c r="AL44" s="26"/>
-      <c r="AM44" s="26"/>
-      <c r="AN44" s="26"/>
-      <c r="AO44" s="26"/>
-      <c r="AP44" s="26"/>
-      <c r="AQ44" s="26"/>
-      <c r="AR44" s="26"/>
-      <c r="AS44" s="26"/>
-      <c r="AT44" s="26"/>
-      <c r="AU44" s="26"/>
-      <c r="AV44" s="26"/>
-      <c r="AW44" s="26"/>
-      <c r="AX44" s="26"/>
-      <c r="AY44" s="26"/>
-      <c r="AZ44" s="26"/>
-      <c r="BA44" s="26"/>
-      <c r="BB44" s="26"/>
-      <c r="BC44" s="26"/>
-      <c r="BD44" s="26"/>
-      <c r="BE44" s="26"/>
-      <c r="BF44" s="26"/>
-      <c r="BG44" s="26"/>
-      <c r="BH44" s="26"/>
-      <c r="BI44" s="26"/>
-      <c r="BJ44" s="26"/>
-      <c r="BK44" s="26"/>
-      <c r="BL44" s="26"/>
-      <c r="BM44" s="26"/>
-      <c r="BN44" s="26"/>
-      <c r="BO44" s="26"/>
-      <c r="BP44" s="26"/>
-      <c r="BQ44" s="26"/>
-      <c r="BR44" s="26"/>
-      <c r="BS44" s="26"/>
-      <c r="BT44" s="26"/>
-      <c r="BU44" s="26"/>
-      <c r="BV44" s="26"/>
-      <c r="BW44" s="26"/>
-      <c r="BX44" s="26"/>
-      <c r="BY44" s="26"/>
-      <c r="BZ44" s="26"/>
+    <row r="44" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="30"/>
+      <c r="C44" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="41">
+        <v>44824</v>
+      </c>
+      <c r="F44" s="41">
+        <v>44835</v>
+      </c>
+      <c r="G44" s="30"/>
+      <c r="H44" s="42">
+        <v>100</v>
+      </c>
+      <c r="I44" s="36"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="32"/>
+      <c r="V44" s="32"/>
+      <c r="W44" s="32"/>
+      <c r="X44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB44" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC44" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD44" s="33"/>
+      <c r="AE44" s="33"/>
+      <c r="AF44" s="33"/>
+      <c r="AG44" s="33"/>
+      <c r="AH44" s="32"/>
+      <c r="AI44" s="32"/>
+      <c r="AJ44" s="32"/>
+      <c r="AK44" s="32"/>
+      <c r="AL44" s="32"/>
+      <c r="AM44" s="32"/>
+      <c r="AN44" s="32"/>
+      <c r="AO44" s="32"/>
+      <c r="AP44" s="32"/>
+      <c r="AQ44" s="32"/>
+      <c r="AR44" s="34"/>
+      <c r="AS44" s="34"/>
+      <c r="AT44" s="34"/>
+      <c r="AU44" s="34"/>
+      <c r="AV44" s="34"/>
+      <c r="AW44" s="32"/>
+      <c r="AX44" s="32"/>
+      <c r="AY44" s="32"/>
+      <c r="AZ44" s="32"/>
+      <c r="BA44" s="32"/>
+      <c r="BB44" s="32"/>
+      <c r="BC44" s="32"/>
+      <c r="BD44" s="32"/>
+      <c r="BE44" s="32"/>
+      <c r="BF44" s="32"/>
+      <c r="BG44" s="35"/>
+      <c r="BH44" s="35"/>
+      <c r="BI44" s="35"/>
+      <c r="BJ44" s="35"/>
+      <c r="BK44" s="35"/>
+      <c r="BL44" s="32"/>
+      <c r="BM44" s="32"/>
+      <c r="BN44" s="32"/>
+      <c r="BO44" s="32"/>
+      <c r="BP44" s="32"/>
+      <c r="BQ44" s="32"/>
+      <c r="BR44" s="32"/>
+      <c r="BS44" s="32"/>
+      <c r="BT44" s="32"/>
+      <c r="BU44" s="32"/>
+      <c r="BV44" s="32"/>
+      <c r="BW44" s="32"/>
+      <c r="BX44" s="32"/>
+      <c r="BY44" s="32"/>
+      <c r="BZ44" s="32"/>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="30">
-        <v>4.0999999999999996</v>
-      </c>
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="30"/>
       <c r="C45" s="44" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E45" s="41">
-        <v>44823</v>
+        <v>44887</v>
       </c>
       <c r="F45" s="41">
-        <v>44825</v>
-      </c>
-      <c r="G45" s="30">
-        <f>DAYS360(E45,F45)</f>
-        <v>2</v>
-      </c>
+        <v>44897</v>
+      </c>
+      <c r="G45" s="30"/>
       <c r="H45" s="42">
         <v>100</v>
       </c>
@@ -5391,12 +5546,8 @@
       <c r="P45" s="38"/>
       <c r="Q45" s="38"/>
       <c r="R45" s="38"/>
-      <c r="S45" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="T45" s="32" t="s">
-        <v>68</v>
-      </c>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
       <c r="U45" s="32"/>
       <c r="V45" s="32"/>
       <c r="W45" s="32"/>
@@ -5441,131 +5592,145 @@
       <c r="BJ45" s="35"/>
       <c r="BK45" s="35"/>
       <c r="BL45" s="32"/>
-      <c r="BM45" s="32"/>
-      <c r="BN45" s="32"/>
-      <c r="BO45" s="32"/>
-      <c r="BP45" s="32"/>
-      <c r="BQ45" s="32"/>
+      <c r="BM45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BN45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BO45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BP45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BQ45" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BR45" s="32"/>
       <c r="BS45" s="32"/>
-      <c r="BT45" s="32"/>
-      <c r="BU45" s="32"/>
-      <c r="BV45" s="32"/>
-      <c r="BW45" s="32"/>
+      <c r="BT45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV45" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW45" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BX45" s="32"/>
       <c r="BY45" s="32"/>
       <c r="BZ45" s="32"/>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="30">
-        <v>4.2</v>
-      </c>
-      <c r="C46" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="30" t="s">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="40">
+        <v>4</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="26"/>
+      <c r="T46" s="26"/>
+      <c r="U46" s="26"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="26"/>
+      <c r="Z46" s="26"/>
+      <c r="AA46" s="26"/>
+      <c r="AB46" s="26"/>
+      <c r="AC46" s="26"/>
+      <c r="AD46" s="26"/>
+      <c r="AE46" s="26"/>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="26"/>
+      <c r="AH46" s="26"/>
+      <c r="AI46" s="26"/>
+      <c r="AJ46" s="26"/>
+      <c r="AK46" s="26"/>
+      <c r="AL46" s="26"/>
+      <c r="AM46" s="26"/>
+      <c r="AN46" s="26"/>
+      <c r="AO46" s="26"/>
+      <c r="AP46" s="26"/>
+      <c r="AQ46" s="26"/>
+      <c r="AR46" s="26"/>
+      <c r="AS46" s="26"/>
+      <c r="AT46" s="26"/>
+      <c r="AU46" s="26"/>
+      <c r="AV46" s="26"/>
+      <c r="AW46" s="26"/>
+      <c r="AX46" s="26"/>
+      <c r="AY46" s="26"/>
+      <c r="AZ46" s="26"/>
+      <c r="BA46" s="26"/>
+      <c r="BB46" s="26"/>
+      <c r="BC46" s="26"/>
+      <c r="BD46" s="26"/>
+      <c r="BE46" s="26"/>
+      <c r="BF46" s="26"/>
+      <c r="BG46" s="26"/>
+      <c r="BH46" s="26"/>
+      <c r="BI46" s="26"/>
+      <c r="BJ46" s="26"/>
+      <c r="BK46" s="26"/>
+      <c r="BL46" s="26"/>
+      <c r="BM46" s="26"/>
+      <c r="BN46" s="26"/>
+      <c r="BO46" s="26"/>
+      <c r="BP46" s="26"/>
+      <c r="BQ46" s="26"/>
+      <c r="BR46" s="26"/>
+      <c r="BS46" s="26"/>
+      <c r="BT46" s="26"/>
+      <c r="BU46" s="26"/>
+      <c r="BV46" s="26"/>
+      <c r="BW46" s="26"/>
+      <c r="BX46" s="26"/>
+      <c r="BY46" s="26"/>
+      <c r="BZ46" s="26"/>
+    </row>
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="30">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C47" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="41">
-        <v>44874</v>
-      </c>
-      <c r="F46" s="41">
-        <v>44876</v>
-      </c>
-      <c r="G46" s="30">
+      <c r="E47" s="41">
+        <v>44823</v>
+      </c>
+      <c r="F47" s="41">
+        <v>44825</v>
+      </c>
+      <c r="G47" s="30">
+        <f>DAYS360(E47,F47)</f>
         <v>2</v>
       </c>
-      <c r="H46" s="42">
+      <c r="H47" s="42">
         <v>100</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="38"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="38"/>
-      <c r="R46" s="38"/>
-      <c r="S46" s="32"/>
-      <c r="T46" s="32"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="32"/>
-      <c r="W46" s="32"/>
-      <c r="X46" s="32"/>
-      <c r="Y46" s="32"/>
-      <c r="Z46" s="32"/>
-      <c r="AA46" s="32"/>
-      <c r="AB46" s="32"/>
-      <c r="AC46" s="33"/>
-      <c r="AD46" s="33"/>
-      <c r="AE46" s="33"/>
-      <c r="AF46" s="33"/>
-      <c r="AG46" s="33"/>
-      <c r="AH46" s="32"/>
-      <c r="AI46" s="32"/>
-      <c r="AJ46" s="32"/>
-      <c r="AK46" s="32"/>
-      <c r="AL46" s="32"/>
-      <c r="AM46" s="32"/>
-      <c r="AN46" s="32"/>
-      <c r="AO46" s="32"/>
-      <c r="AP46" s="32"/>
-      <c r="AQ46" s="32"/>
-      <c r="AR46" s="34"/>
-      <c r="AS46" s="34"/>
-      <c r="AT46" s="34"/>
-      <c r="AU46" s="34"/>
-      <c r="AV46" s="34"/>
-      <c r="AW46" s="32"/>
-      <c r="AX46" s="32"/>
-      <c r="AY46" s="32"/>
-      <c r="AZ46" s="32"/>
-      <c r="BA46" s="32"/>
-      <c r="BB46" s="32"/>
-      <c r="BC46" s="32"/>
-      <c r="BD46" s="32"/>
-      <c r="BE46" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="BF46" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="BG46" s="35"/>
-      <c r="BH46" s="35"/>
-      <c r="BI46" s="35"/>
-      <c r="BJ46" s="35"/>
-      <c r="BK46" s="35"/>
-      <c r="BL46" s="32"/>
-      <c r="BM46" s="32"/>
-      <c r="BN46" s="32"/>
-      <c r="BO46" s="32"/>
-      <c r="BP46" s="32"/>
-      <c r="BQ46" s="32"/>
-      <c r="BR46" s="32"/>
-      <c r="BS46" s="32"/>
-      <c r="BT46" s="32"/>
-      <c r="BU46" s="32"/>
-      <c r="BV46" s="32"/>
-      <c r="BW46" s="32"/>
-      <c r="BX46" s="32"/>
-      <c r="BY46" s="32"/>
-      <c r="BZ46" s="32"/>
-    </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="30">
-        <f t="shared" ref="G47:G49" si="5">DAYS360(E47,F47)</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="31"/>
       <c r="I47" s="36"/>
       <c r="J47" s="37"/>
       <c r="K47" s="32"/>
@@ -5576,8 +5741,12 @@
       <c r="P47" s="38"/>
       <c r="Q47" s="38"/>
       <c r="R47" s="38"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
+      <c r="S47" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="T47" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="U47" s="32"/>
       <c r="V47" s="32"/>
       <c r="W47" s="32"/>
@@ -5637,19 +5806,28 @@
       <c r="BY47" s="32"/>
       <c r="BZ47" s="32"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="30">
+        <v>4.2</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="41">
+        <v>44874</v>
+      </c>
+      <c r="F48" s="41">
+        <v>44876</v>
+      </c>
       <c r="G48" s="30">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="42"/>
+        <v>2</v>
+      </c>
+      <c r="H48" s="42">
+        <v>100</v>
+      </c>
       <c r="I48" s="36"/>
       <c r="J48" s="37"/>
       <c r="K48" s="32"/>
@@ -5698,8 +5876,12 @@
       <c r="BB48" s="32"/>
       <c r="BC48" s="32"/>
       <c r="BD48" s="32"/>
-      <c r="BE48" s="32"/>
-      <c r="BF48" s="32"/>
+      <c r="BE48" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF48" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="BG48" s="35"/>
       <c r="BH48" s="35"/>
       <c r="BI48" s="35"/>
@@ -5721,16 +5903,16 @@
       <c r="BY48" s="32"/>
       <c r="BZ48" s="32"/>
     </row>
-    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="30">
-        <v>4.3</v>
+    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="30"/>
       <c r="E49" s="41"/>
       <c r="F49" s="41"/>
       <c r="G49" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G49:G51" si="5">DAYS360(E49,F49)</f>
         <v>0</v>
       </c>
       <c r="H49" s="31"/>
@@ -5805,18 +5987,19 @@
       <c r="BY49" s="32"/>
       <c r="BZ49" s="32"/>
     </row>
-    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="46"/>
+        <v>42</v>
+      </c>
+      <c r="C50" s="44"/>
       <c r="D50" s="30"/>
       <c r="E50" s="41"/>
       <c r="F50" s="41"/>
       <c r="G50" s="30">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H50" s="31"/>
+      <c r="H50" s="42"/>
       <c r="I50" s="36"/>
       <c r="J50" s="37"/>
       <c r="K50" s="32"/>
@@ -5888,8 +6071,195 @@
       <c r="BY50" s="32"/>
       <c r="BZ50" s="32"/>
     </row>
+    <row r="51" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="C51" s="44"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="31"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="38"/>
+      <c r="O51" s="38"/>
+      <c r="P51" s="38"/>
+      <c r="Q51" s="38"/>
+      <c r="R51" s="38"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="32"/>
+      <c r="V51" s="32"/>
+      <c r="W51" s="32"/>
+      <c r="X51" s="32"/>
+      <c r="Y51" s="32"/>
+      <c r="Z51" s="32"/>
+      <c r="AA51" s="32"/>
+      <c r="AB51" s="32"/>
+      <c r="AC51" s="33"/>
+      <c r="AD51" s="33"/>
+      <c r="AE51" s="33"/>
+      <c r="AF51" s="33"/>
+      <c r="AG51" s="33"/>
+      <c r="AH51" s="32"/>
+      <c r="AI51" s="32"/>
+      <c r="AJ51" s="32"/>
+      <c r="AK51" s="32"/>
+      <c r="AL51" s="32"/>
+      <c r="AM51" s="32"/>
+      <c r="AN51" s="32"/>
+      <c r="AO51" s="32"/>
+      <c r="AP51" s="32"/>
+      <c r="AQ51" s="32"/>
+      <c r="AR51" s="34"/>
+      <c r="AS51" s="34"/>
+      <c r="AT51" s="34"/>
+      <c r="AU51" s="34"/>
+      <c r="AV51" s="34"/>
+      <c r="AW51" s="32"/>
+      <c r="AX51" s="32"/>
+      <c r="AY51" s="32"/>
+      <c r="AZ51" s="32"/>
+      <c r="BA51" s="32"/>
+      <c r="BB51" s="32"/>
+      <c r="BC51" s="32"/>
+      <c r="BD51" s="32"/>
+      <c r="BE51" s="32"/>
+      <c r="BF51" s="32"/>
+      <c r="BG51" s="35"/>
+      <c r="BH51" s="35"/>
+      <c r="BI51" s="35"/>
+      <c r="BJ51" s="35"/>
+      <c r="BK51" s="35"/>
+      <c r="BL51" s="32"/>
+      <c r="BM51" s="32"/>
+      <c r="BN51" s="32"/>
+      <c r="BO51" s="32"/>
+      <c r="BP51" s="32"/>
+      <c r="BQ51" s="32"/>
+      <c r="BR51" s="32"/>
+      <c r="BS51" s="32"/>
+      <c r="BT51" s="32"/>
+      <c r="BU51" s="32"/>
+      <c r="BV51" s="32"/>
+      <c r="BW51" s="32"/>
+      <c r="BX51" s="32"/>
+      <c r="BY51" s="32"/>
+      <c r="BZ51" s="32"/>
+    </row>
+    <row r="52" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="46"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="30">
+        <v>0</v>
+      </c>
+      <c r="H52" s="31"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="32"/>
+      <c r="V52" s="32"/>
+      <c r="W52" s="32"/>
+      <c r="X52" s="32"/>
+      <c r="Y52" s="32"/>
+      <c r="Z52" s="32"/>
+      <c r="AA52" s="32"/>
+      <c r="AB52" s="32"/>
+      <c r="AC52" s="33"/>
+      <c r="AD52" s="33"/>
+      <c r="AE52" s="33"/>
+      <c r="AF52" s="33"/>
+      <c r="AG52" s="33"/>
+      <c r="AH52" s="32"/>
+      <c r="AI52" s="32"/>
+      <c r="AJ52" s="32"/>
+      <c r="AK52" s="32"/>
+      <c r="AL52" s="32"/>
+      <c r="AM52" s="32"/>
+      <c r="AN52" s="32"/>
+      <c r="AO52" s="32"/>
+      <c r="AP52" s="32"/>
+      <c r="AQ52" s="32"/>
+      <c r="AR52" s="34"/>
+      <c r="AS52" s="34"/>
+      <c r="AT52" s="34"/>
+      <c r="AU52" s="34"/>
+      <c r="AV52" s="34"/>
+      <c r="AW52" s="32"/>
+      <c r="AX52" s="32"/>
+      <c r="AY52" s="32"/>
+      <c r="AZ52" s="32"/>
+      <c r="BA52" s="32"/>
+      <c r="BB52" s="32"/>
+      <c r="BC52" s="32"/>
+      <c r="BD52" s="32"/>
+      <c r="BE52" s="32"/>
+      <c r="BF52" s="32"/>
+      <c r="BG52" s="35"/>
+      <c r="BH52" s="35"/>
+      <c r="BI52" s="35"/>
+      <c r="BJ52" s="35"/>
+      <c r="BK52" s="35"/>
+      <c r="BL52" s="32"/>
+      <c r="BM52" s="32"/>
+      <c r="BN52" s="32"/>
+      <c r="BO52" s="32"/>
+      <c r="BP52" s="32"/>
+      <c r="BQ52" s="32"/>
+      <c r="BR52" s="32"/>
+      <c r="BS52" s="32"/>
+      <c r="BT52" s="32"/>
+      <c r="BU52" s="32"/>
+      <c r="BV52" s="32"/>
+      <c r="BW52" s="32"/>
+      <c r="BX52" s="32"/>
+      <c r="BY52" s="32"/>
+      <c r="BZ52" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -5906,29 +6276,9 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
   </mergeCells>
-  <conditionalFormatting sqref="H11:H14 H16:H50">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="H11:H14 H16:H52">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5937,8 +6287,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H14 H16:H50">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="H11:H14 H16:H52">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5953,9 +6303,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6188,27 +6541,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6233,9 +6574,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add comments SnakeGame, Update Gantt
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt.xlsx
+++ b/docs/gantt/Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unreal\CPS353-01-Moon-Game\CPS353-01-Moon-Game\docs\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\CPS353-01-Moon-Game\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080C9261-65AA-4F2D-86FB-742FC1E49909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F063E184-587D-4367-9F66-82A10A5C9BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="87">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -855,8 +855,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -874,14 +903,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -893,30 +917,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,7 +936,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1300,22 +1300,22 @@
   </sheetPr>
   <dimension ref="A1:BZ54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" customWidth="1"/>
-    <col min="3" max="3" width="31.73046875" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.86328125" customWidth="1"/>
-    <col min="9" max="78" width="3.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="9" max="78" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1395,40 +1395,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1477,7 +1477,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1557,13 +1557,13 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="1.1000000000000001">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="55"/>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="65" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="57"/>
@@ -1579,7 +1579,7 @@
       <c r="M4" s="55"/>
       <c r="N4" s="55"/>
       <c r="O4" s="55"/>
-      <c r="P4" s="58" t="s">
+      <c r="P4" s="66" t="s">
         <v>2</v>
       </c>
       <c r="Q4" s="57"/>
@@ -1645,13 +1645,13 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="54" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="55"/>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="56" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="57"/>
@@ -1667,7 +1667,7 @@
       <c r="M5" s="55"/>
       <c r="N5" s="55"/>
       <c r="O5" s="55"/>
-      <c r="P5" s="69">
+      <c r="P5" s="58">
         <v>44802</v>
       </c>
       <c r="Q5" s="57"/>
@@ -1733,7 +1733,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="22" t="s">
         <v>46</v>
@@ -1815,7 +1815,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -1895,209 +1895,209 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62"/>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="62"/>
-      <c r="AE8" s="62"/>
-      <c r="AF8" s="62"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="62"/>
-      <c r="AI8" s="62"/>
-      <c r="AJ8" s="62"/>
-      <c r="AK8" s="62"/>
-      <c r="AL8" s="62"/>
-      <c r="AM8" s="63"/>
-      <c r="AN8" s="62"/>
-      <c r="AO8" s="62"/>
-      <c r="AP8" s="62"/>
-      <c r="AQ8" s="62"/>
-      <c r="AR8" s="62"/>
-      <c r="AS8" s="62"/>
-      <c r="AT8" s="62"/>
-      <c r="AU8" s="62"/>
-      <c r="AV8" s="62"/>
-      <c r="AW8" s="62"/>
-      <c r="AX8" s="62"/>
-      <c r="AY8" s="62"/>
-      <c r="AZ8" s="62"/>
-      <c r="BA8" s="62"/>
-      <c r="BB8" s="63"/>
-      <c r="BC8" s="62"/>
-      <c r="BD8" s="62"/>
-      <c r="BE8" s="62"/>
-      <c r="BF8" s="62"/>
-      <c r="BG8" s="62"/>
-      <c r="BH8" s="62"/>
-      <c r="BI8" s="62"/>
-      <c r="BJ8" s="62"/>
-      <c r="BK8" s="62"/>
-      <c r="BL8" s="62"/>
-      <c r="BM8" s="62"/>
-      <c r="BN8" s="62"/>
-      <c r="BO8" s="62"/>
-      <c r="BP8" s="62"/>
-      <c r="BQ8" s="62"/>
-      <c r="BR8" s="62"/>
-      <c r="BS8" s="62"/>
-      <c r="BT8" s="62"/>
-      <c r="BU8" s="62"/>
-      <c r="BV8" s="62"/>
-      <c r="BW8" s="62"/>
-      <c r="BX8" s="62"/>
-      <c r="BY8" s="62"/>
-      <c r="BZ8" s="67"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="48"/>
+      <c r="AN8" s="49"/>
+      <c r="AO8" s="49"/>
+      <c r="AP8" s="49"/>
+      <c r="AQ8" s="49"/>
+      <c r="AR8" s="49"/>
+      <c r="AS8" s="49"/>
+      <c r="AT8" s="49"/>
+      <c r="AU8" s="49"/>
+      <c r="AV8" s="49"/>
+      <c r="AW8" s="49"/>
+      <c r="AX8" s="49"/>
+      <c r="AY8" s="49"/>
+      <c r="AZ8" s="49"/>
+      <c r="BA8" s="49"/>
+      <c r="BB8" s="48"/>
+      <c r="BC8" s="49"/>
+      <c r="BD8" s="49"/>
+      <c r="BE8" s="49"/>
+      <c r="BF8" s="49"/>
+      <c r="BG8" s="49"/>
+      <c r="BH8" s="49"/>
+      <c r="BI8" s="49"/>
+      <c r="BJ8" s="49"/>
+      <c r="BK8" s="49"/>
+      <c r="BL8" s="49"/>
+      <c r="BM8" s="49"/>
+      <c r="BN8" s="49"/>
+      <c r="BO8" s="49"/>
+      <c r="BP8" s="49"/>
+      <c r="BQ8" s="49"/>
+      <c r="BR8" s="49"/>
+      <c r="BS8" s="49"/>
+      <c r="BT8" s="49"/>
+      <c r="BU8" s="49"/>
+      <c r="BV8" s="49"/>
+      <c r="BW8" s="49"/>
+      <c r="BX8" s="49"/>
+      <c r="BY8" s="49"/>
+      <c r="BZ8" s="50"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="64" t="s">
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="64" t="s">
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="64" t="s">
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="65"/>
-      <c r="U9" s="65"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="64" t="s">
+      <c r="T9" s="52"/>
+      <c r="U9" s="52"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="66"/>
-      <c r="AC9" s="64" t="s">
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="53"/>
+      <c r="AC9" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="65"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="66"/>
-      <c r="AH9" s="64" t="s">
+      <c r="AD9" s="52"/>
+      <c r="AE9" s="52"/>
+      <c r="AF9" s="52"/>
+      <c r="AG9" s="53"/>
+      <c r="AH9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="AI9" s="65"/>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="65"/>
-      <c r="AL9" s="66"/>
-      <c r="AM9" s="64" t="s">
+      <c r="AI9" s="52"/>
+      <c r="AJ9" s="52"/>
+      <c r="AK9" s="52"/>
+      <c r="AL9" s="53"/>
+      <c r="AM9" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="65"/>
-      <c r="AP9" s="65"/>
-      <c r="AQ9" s="66"/>
-      <c r="AR9" s="64" t="s">
+      <c r="AN9" s="52"/>
+      <c r="AO9" s="52"/>
+      <c r="AP9" s="52"/>
+      <c r="AQ9" s="53"/>
+      <c r="AR9" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AS9" s="65"/>
-      <c r="AT9" s="65"/>
-      <c r="AU9" s="65"/>
-      <c r="AV9" s="66"/>
-      <c r="AW9" s="64" t="s">
+      <c r="AS9" s="52"/>
+      <c r="AT9" s="52"/>
+      <c r="AU9" s="52"/>
+      <c r="AV9" s="53"/>
+      <c r="AW9" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="AX9" s="65"/>
-      <c r="AY9" s="65"/>
-      <c r="AZ9" s="65"/>
-      <c r="BA9" s="66"/>
-      <c r="BB9" s="64" t="s">
+      <c r="AX9" s="52"/>
+      <c r="AY9" s="52"/>
+      <c r="AZ9" s="52"/>
+      <c r="BA9" s="53"/>
+      <c r="BB9" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="BC9" s="65"/>
-      <c r="BD9" s="65"/>
-      <c r="BE9" s="65"/>
-      <c r="BF9" s="66"/>
-      <c r="BG9" s="64" t="s">
+      <c r="BC9" s="52"/>
+      <c r="BD9" s="52"/>
+      <c r="BE9" s="52"/>
+      <c r="BF9" s="53"/>
+      <c r="BG9" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="BH9" s="65"/>
-      <c r="BI9" s="65"/>
-      <c r="BJ9" s="65"/>
-      <c r="BK9" s="66"/>
-      <c r="BL9" s="64" t="s">
+      <c r="BH9" s="52"/>
+      <c r="BI9" s="52"/>
+      <c r="BJ9" s="52"/>
+      <c r="BK9" s="53"/>
+      <c r="BL9" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="BM9" s="65"/>
-      <c r="BN9" s="65"/>
-      <c r="BO9" s="65"/>
-      <c r="BP9" s="66"/>
-      <c r="BQ9" s="64" t="s">
+      <c r="BM9" s="52"/>
+      <c r="BN9" s="52"/>
+      <c r="BO9" s="52"/>
+      <c r="BP9" s="53"/>
+      <c r="BQ9" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="BR9" s="65"/>
-      <c r="BS9" s="65"/>
-      <c r="BT9" s="65"/>
-      <c r="BU9" s="66"/>
-      <c r="BV9" s="64" t="s">
+      <c r="BR9" s="52"/>
+      <c r="BS9" s="52"/>
+      <c r="BT9" s="52"/>
+      <c r="BU9" s="53"/>
+      <c r="BV9" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="BW9" s="65"/>
-      <c r="BX9" s="65"/>
-      <c r="BY9" s="65"/>
-      <c r="BZ9" s="66"/>
+      <c r="BW9" s="52"/>
+      <c r="BX9" s="52"/>
+      <c r="BY9" s="52"/>
+      <c r="BZ9" s="53"/>
     </row>
-    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="40">
         <v>1</v>
@@ -2181,7 +2181,7 @@
       <c r="BY10" s="26"/>
       <c r="BZ10" s="26"/>
     </row>
-    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="30">
         <v>1.1000000000000001</v>
@@ -2276,7 +2276,7 @@
       <c r="BY11" s="32"/>
       <c r="BZ11" s="32"/>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
         <v>13</v>
@@ -2371,7 +2371,7 @@
       <c r="BY12" s="32"/>
       <c r="BZ12" s="32"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
       <c r="B13" s="30">
         <v>1.2</v>
@@ -2466,7 +2466,7 @@
       <c r="BY13" s="32"/>
       <c r="BZ13" s="32"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="30">
         <v>1.3</v>
@@ -2561,7 +2561,7 @@
       <c r="BY14" s="32"/>
       <c r="BZ14" s="32"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="40">
         <v>2</v>
@@ -2645,7 +2645,7 @@
       <c r="BY15" s="26"/>
       <c r="BZ15" s="26"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="30">
         <v>2.1</v>
@@ -2755,7 +2755,7 @@
       <c r="BY16" s="32"/>
       <c r="BZ16" s="32"/>
     </row>
-    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="30">
         <v>2.2999999999999998</v>
@@ -2870,7 +2870,7 @@
       <c r="BY17" s="32"/>
       <c r="BZ17" s="32"/>
     </row>
-    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
@@ -2978,7 +2978,7 @@
       <c r="BY18" s="32"/>
       <c r="BZ18" s="32"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="30">
         <v>2.5</v>
@@ -3089,7 +3089,7 @@
       <c r="BY19" s="32"/>
       <c r="BZ19" s="32"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="30">
         <v>2.6</v>
@@ -3209,7 +3209,7 @@
       <c r="BY20" s="32"/>
       <c r="BZ20" s="32"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="30">
         <v>2.2000000000000002</v>
@@ -3298,7 +3298,7 @@
       <c r="BY21" s="32"/>
       <c r="BZ21" s="32"/>
     </row>
-    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="30">
         <v>2.7</v>
@@ -3385,7 +3385,7 @@
       <c r="BY22" s="32"/>
       <c r="BZ22" s="32"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="30">
         <v>2.8</v>
@@ -3470,7 +3470,7 @@
       <c r="BY23" s="32"/>
       <c r="BZ23" s="32"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="30">
         <v>2.9</v>
@@ -3554,7 +3554,7 @@
       <c r="BY24" s="32"/>
       <c r="BZ24" s="32"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="30">
         <v>2.4</v>
@@ -3643,7 +3643,7 @@
       <c r="BY25" s="32"/>
       <c r="BZ25" s="32"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
       <c r="B26" s="45">
         <v>2.1</v>
@@ -3728,7 +3728,7 @@
       <c r="BY26" s="32"/>
       <c r="BZ26" s="32"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="45">
         <v>2.11</v>
@@ -3812,7 +3812,7 @@
       <c r="BY27" s="32"/>
       <c r="BZ27" s="32"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="40">
         <v>3</v>
@@ -3896,7 +3896,7 @@
       <c r="BY28" s="26"/>
       <c r="BZ28" s="26"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="30">
         <v>3.1</v>
@@ -3985,7 +3985,7 @@
       <c r="BY29" s="32"/>
       <c r="BZ29" s="32"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="30">
         <v>3.2</v>
@@ -4073,7 +4073,7 @@
       <c r="BY30" s="32"/>
       <c r="BZ30" s="32"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="30" t="s">
         <v>17</v>
@@ -4172,10 +4172,12 @@
       </c>
       <c r="BW31" s="32"/>
       <c r="BX31" s="32"/>
-      <c r="BY31" s="32"/>
+      <c r="BY31" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BZ31" s="32"/>
     </row>
-    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="30" t="s">
         <v>18</v>
@@ -4194,7 +4196,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="42">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I32" s="36"/>
       <c r="J32" s="37"/>
@@ -4294,10 +4296,12 @@
       <c r="BX32" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="BY32" s="32"/>
+      <c r="BY32" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BZ32" s="32"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="30">
         <v>3.3</v>
@@ -4394,10 +4398,12 @@
       <c r="BX33" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="BY33" s="32"/>
+      <c r="BY33" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BZ33" s="32"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="30" t="s">
         <v>19</v>
@@ -4514,10 +4520,12 @@
       <c r="BX34" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="BY34" s="32"/>
+      <c r="BY34" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BZ34" s="32"/>
     </row>
-    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
       <c r="C35" s="44" t="s">
         <v>67</v>
@@ -4629,10 +4637,12 @@
       <c r="BX35" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="BY35" s="32"/>
+      <c r="BY35" s="32" t="s">
+        <v>68</v>
+      </c>
       <c r="BZ35" s="32"/>
     </row>
-    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="43" t="s">
@@ -4734,7 +4744,7 @@
       <c r="BY36" s="32"/>
       <c r="BZ36" s="32"/>
     </row>
-    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="C37" s="44" t="s">
         <v>72</v>
@@ -4853,7 +4863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" s="44" t="s">
         <v>73</v>
@@ -4970,7 +4980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="44" t="s">
@@ -5119,7 +5129,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
       <c r="C40" s="44" t="s">
         <v>66</v>
@@ -5232,7 +5242,7 @@
       <c r="BY40" s="32"/>
       <c r="BZ40" s="32"/>
     </row>
-    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="44" t="s">
@@ -5346,7 +5356,7 @@
       <c r="BY41" s="32"/>
       <c r="BZ41" s="32"/>
     </row>
-    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="44" t="s">
@@ -5433,7 +5443,7 @@
       <c r="BY42" s="32"/>
       <c r="BZ42" s="32"/>
     </row>
-    <row r="43" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
       <c r="C43" s="44" t="s">
@@ -5535,7 +5545,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
       <c r="C44" s="44" t="s">
@@ -5652,7 +5662,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
       <c r="C45" s="44" t="s">
         <v>65</v>
@@ -5771,7 +5781,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
       <c r="C46" s="44" t="s">
         <v>83</v>
@@ -5872,7 +5882,7 @@
       <c r="BY46" s="32"/>
       <c r="BZ46" s="32"/>
     </row>
-    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="30"/>
       <c r="C47" s="44" t="s">
         <v>84</v>
@@ -5979,7 +5989,7 @@
       <c r="BY47" s="32"/>
       <c r="BZ47" s="32"/>
     </row>
-    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="40">
         <v>4</v>
       </c>
@@ -6062,7 +6072,7 @@
       <c r="BY48" s="26"/>
       <c r="BZ48" s="26"/>
     </row>
-    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="30">
         <v>4.0999999999999996</v>
       </c>
@@ -6160,7 +6170,7 @@
       <c r="BY49" s="32"/>
       <c r="BZ49" s="32"/>
     </row>
-    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="30">
         <v>4.2</v>
       </c>
@@ -6257,7 +6267,7 @@
       <c r="BY50" s="32"/>
       <c r="BZ50" s="32"/>
     </row>
-    <row r="51" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="30" t="s">
         <v>41</v>
       </c>
@@ -6341,7 +6351,7 @@
       <c r="BY51" s="32"/>
       <c r="BZ51" s="32"/>
     </row>
-    <row r="52" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="30" t="s">
         <v>42</v>
       </c>
@@ -6425,7 +6435,7 @@
       <c r="BY52" s="32"/>
       <c r="BZ52" s="32"/>
     </row>
-    <row r="53" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="30">
         <v>4.3</v>
       </c>
@@ -6509,7 +6519,7 @@
       <c r="BY53" s="32"/>
       <c r="BZ53" s="32"/>
     </row>
-    <row r="54" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="30" t="s">
         <v>43</v>
       </c>
@@ -6594,6 +6604,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
     <mergeCell ref="BB8:BZ8"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:R9"/>
@@ -6610,26 +6640,6 @@
     <mergeCell ref="BQ9:BU9"/>
     <mergeCell ref="BV9:BZ9"/>
     <mergeCell ref="S9:W9"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H14 H16:H54">
     <cfRule type="colorScale" priority="26">
@@ -6657,12 +6667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7EF2104F2CEFE4DACFBF5BA7D93FB4D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb0ed258f694207805e211ca255f9b46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b71f768-6d8b-468c-a986-1e1afc74f0e3" xmlns:ns4="d07d918a-d172-4450-8f4a-7b087689ff85" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c03c9fe975be0719773112499dde791" ns3:_="" ns4:_="">
     <xsd:import namespace="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
@@ -6891,6 +6895,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6901,23 +6911,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FABC364-430D-422C-AD85-145699D2125C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6936,6 +6929,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>

</xml_diff>